<commit_message>
feat: run top 1-5%
</commit_message>
<xml_diff>
--- a/results/01_annotations/Supplementary_Table2.xlsx
+++ b/results/01_annotations/Supplementary_Table2.xlsx
@@ -13,7 +13,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="41" uniqueCount="41">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="43" uniqueCount="43">
   <si>
     <t xml:space="preserve">Column name</t>
   </si>
@@ -108,7 +108,7 @@
     <t xml:space="preserve">AD2019</t>
   </si>
   <si>
-    <t xml:space="preserve">Top 0.5%</t>
+    <t xml:space="preserve">Top 1%</t>
   </si>
   <si>
     <t xml:space="preserve">CLR</t>
@@ -126,10 +126,16 @@
     <t xml:space="preserve">XPEHH</t>
   </si>
   <si>
-    <t xml:space="preserve">Top 1%</t>
-  </si>
-  <si>
     <t xml:space="preserve">Top 2%</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Top 3%</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Top 4%</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Top 5%</t>
   </si>
   <si>
     <t xml:space="preserve">ALS2021.EUR</t>
@@ -667,37 +673,37 @@
         <v>32</v>
       </c>
       <c r="D2" t="n">
-        <v>0.00365113562648</v>
+        <v>0.00799609606119</v>
       </c>
       <c r="E2" t="n">
-        <v>-0.000504817995284</v>
+        <v>-0.00229968889921</v>
       </c>
       <c r="F2" t="n">
-        <v>0.00215479787028</v>
+        <v>0.00282474344873</v>
       </c>
       <c r="G2" t="n">
-        <v>-0.138263282148</v>
+        <v>-0.287601459714</v>
       </c>
       <c r="H2" t="n">
-        <v>0.590171960377</v>
+        <v>0.353265321866</v>
       </c>
       <c r="I2" t="n">
-        <v>0.0519734303206095</v>
+        <v>0.00026276465990583</v>
       </c>
       <c r="J2" t="n">
-        <v>-0.00000000111491295829</v>
+        <v>-0.00000000148052839863</v>
       </c>
       <c r="K2" t="n">
-        <v>0.00000000159443153691</v>
+        <v>0.000000000908612360895</v>
       </c>
       <c r="L2" t="n">
-        <v>-0.699254205956</v>
+        <v>-1.62943898009</v>
       </c>
       <c r="M2" t="n">
-        <v>0.484393180246413</v>
+        <v>0.1032201225732</v>
       </c>
       <c r="N2" t="n">
-        <v>0.660536154881473</v>
+        <v>0.405512845618418</v>
       </c>
     </row>
     <row r="3">
@@ -711,37 +717,37 @@
         <v>33</v>
       </c>
       <c r="D3" t="n">
-        <v>0.00434177313506</v>
+        <v>0.00866542898789</v>
       </c>
       <c r="E3" t="n">
-        <v>0.00282778964456</v>
+        <v>0.00853701405276</v>
       </c>
       <c r="F3" t="n">
-        <v>0.00772570017459</v>
+        <v>0.0105391125451</v>
       </c>
       <c r="G3" t="n">
-        <v>0.651298342082</v>
+        <v>0.985180775781</v>
       </c>
       <c r="H3" t="n">
-        <v>1.77938826702</v>
+        <v>1.21622513552</v>
       </c>
       <c r="I3" t="n">
-        <v>0.845104830297791</v>
+        <v>0.990286009389119</v>
       </c>
       <c r="J3" t="n">
-        <v>-0.0000000012535256394</v>
+        <v>-0.000000000370572935372</v>
       </c>
       <c r="K3" t="n">
-        <v>0.00000000484249720481</v>
+        <v>0.00000000330349002936</v>
       </c>
       <c r="L3" t="n">
-        <v>-0.25885934186</v>
+        <v>-0.11217619308</v>
       </c>
       <c r="M3" t="n">
-        <v>0.795743769638983</v>
+        <v>0.910683705181684</v>
       </c>
       <c r="N3" t="n">
-        <v>0.852582610327482</v>
+        <v>0.910683705181684</v>
       </c>
     </row>
     <row r="4">
@@ -755,37 +761,37 @@
         <v>34</v>
       </c>
       <c r="D4" t="n">
-        <v>0.00566886405815</v>
+        <v>0.0113685945971</v>
       </c>
       <c r="E4" t="n">
-        <v>-0.00741826279294</v>
+        <v>-0.0212840979099</v>
       </c>
       <c r="F4" t="n">
-        <v>0.0189325519459</v>
+        <v>0.0243515154304</v>
       </c>
       <c r="G4" t="n">
-        <v>-1.3085977573</v>
+        <v>-1.87218373635</v>
       </c>
       <c r="H4" t="n">
-        <v>3.33974350976</v>
+        <v>2.14199875124</v>
       </c>
       <c r="I4" t="n">
-        <v>0.490667267241791</v>
+        <v>0.185412662623881</v>
       </c>
       <c r="J4" t="n">
-        <v>-0.00000000567124935075</v>
+        <v>-0.00000000729321027458</v>
       </c>
       <c r="K4" t="n">
-        <v>0.00000000918003810157</v>
+        <v>0.00000000590121810634</v>
       </c>
       <c r="L4" t="n">
-        <v>-0.617780589579</v>
+        <v>-1.23588217604</v>
       </c>
       <c r="M4" t="n">
-        <v>0.536719980147297</v>
+        <v>0.216502363284875</v>
       </c>
       <c r="N4" t="n">
-        <v>0.670899975184121</v>
+        <v>0.520473437307806</v>
       </c>
     </row>
     <row r="5">
@@ -799,37 +805,37 @@
         <v>35</v>
       </c>
       <c r="D5" t="n">
-        <v>0.00551050559128</v>
+        <v>0.0111318956599</v>
       </c>
       <c r="E5" t="n">
-        <v>0.00355211893848</v>
+        <v>0.00649428781169</v>
       </c>
       <c r="F5" t="n">
-        <v>0.00423250099673</v>
+        <v>0.00684249483682</v>
       </c>
       <c r="G5" t="n">
-        <v>0.644608535396</v>
+        <v>0.583394599636</v>
       </c>
       <c r="H5" t="n">
-        <v>0.768078523217</v>
+        <v>0.614674719013</v>
       </c>
       <c r="I5" t="n">
-        <v>0.649240147769815</v>
+        <v>0.500547330686165</v>
       </c>
       <c r="J5" t="n">
-        <v>-0.00000000167118517191</v>
+        <v>-0.00000000149555633</v>
       </c>
       <c r="K5" t="n">
-        <v>0.00000000223036828395</v>
+        <v>0.00000000176865901165</v>
       </c>
       <c r="L5" t="n">
-        <v>-0.749286646488</v>
+        <v>-0.84558771371</v>
       </c>
       <c r="M5" t="n">
-        <v>0.453684454558011</v>
+        <v>0.397782781925568</v>
       </c>
       <c r="N5" t="n">
-        <v>0.660536154881473</v>
+        <v>0.63497534077209</v>
       </c>
     </row>
     <row r="6">
@@ -843,37 +849,37 @@
         <v>36</v>
       </c>
       <c r="D6" t="n">
-        <v>0.00451170653224</v>
+        <v>0.0091354718101</v>
       </c>
       <c r="E6" t="n">
-        <v>-0.00504754220404</v>
+        <v>-0.00698254583635</v>
       </c>
       <c r="F6" t="n">
-        <v>0.00629414350435</v>
+        <v>0.0104115983706</v>
       </c>
       <c r="G6" t="n">
-        <v>-1.11876563069</v>
+        <v>-0.764333356995</v>
       </c>
       <c r="H6" t="n">
-        <v>1.39506935112</v>
+        <v>1.13968917939</v>
       </c>
       <c r="I6" t="n">
-        <v>0.131101358852598</v>
+        <v>0.121840005509611</v>
       </c>
       <c r="J6" t="n">
-        <v>-0.00000000421317318709</v>
+        <v>-0.00000000357689877979</v>
       </c>
       <c r="K6" t="n">
-        <v>0.0000000040553678057</v>
+        <v>0.00000000340028042235</v>
       </c>
       <c r="L6" t="n">
-        <v>-1.0389127174</v>
+        <v>-1.05194229166</v>
       </c>
       <c r="M6" t="n">
-        <v>0.298845331254992</v>
+        <v>0.292826026955575</v>
       </c>
       <c r="N6" t="n">
-        <v>0.560334996103109</v>
+        <v>0.563126974914567</v>
       </c>
     </row>
     <row r="7">
@@ -887,37 +893,37 @@
         <v>32</v>
       </c>
       <c r="D7" t="n">
-        <v>0.00799609606119</v>
+        <v>0.0158392017391</v>
       </c>
       <c r="E7" t="n">
-        <v>-0.00229968889921</v>
+        <v>-0.00735995181753</v>
       </c>
       <c r="F7" t="n">
-        <v>0.00282474344873</v>
+        <v>0.00485251854032</v>
       </c>
       <c r="G7" t="n">
-        <v>-0.287601459714</v>
+        <v>-0.464666839829</v>
       </c>
       <c r="H7" t="n">
-        <v>0.353265321866</v>
+        <v>0.306361306601</v>
       </c>
       <c r="I7" t="n">
-        <v>0.00026276465990583</v>
+        <v>0.000000382613149869517</v>
       </c>
       <c r="J7" t="n">
-        <v>-0.00000000148052839863</v>
+        <v>-0.00000000212125136724</v>
       </c>
       <c r="K7" t="n">
-        <v>0.000000000908612360895</v>
+        <v>0.00000000070783657823</v>
       </c>
       <c r="L7" t="n">
-        <v>-1.62943898009</v>
+        <v>-2.99680947903</v>
       </c>
       <c r="M7" t="n">
-        <v>0.1032201225732</v>
+        <v>0.00272821159936071</v>
       </c>
       <c r="N7" t="n">
-        <v>0.560334996103109</v>
+        <v>0.0230339501796225</v>
       </c>
     </row>
     <row r="8">
@@ -931,37 +937,37 @@
         <v>33</v>
       </c>
       <c r="D8" t="n">
-        <v>0.00866542898789</v>
+        <v>0.0170143087946</v>
       </c>
       <c r="E8" t="n">
-        <v>0.00853701405276</v>
+        <v>0.0115885684388</v>
       </c>
       <c r="F8" t="n">
-        <v>0.0105391125451</v>
+        <v>0.0142802161307</v>
       </c>
       <c r="G8" t="n">
-        <v>0.985180775781</v>
+        <v>0.681107212677</v>
       </c>
       <c r="H8" t="n">
-        <v>1.21622513552</v>
+        <v>0.839306274679</v>
       </c>
       <c r="I8" t="n">
-        <v>0.990286009389119</v>
+        <v>0.704635420890283</v>
       </c>
       <c r="J8" t="n">
-        <v>-0.000000000370572935372</v>
+        <v>-0.00000000124476254202</v>
       </c>
       <c r="K8" t="n">
-        <v>0.00000000330349002936</v>
+        <v>0.00000000231367042723</v>
       </c>
       <c r="L8" t="n">
-        <v>-0.11217619308</v>
+        <v>-0.538003393817</v>
       </c>
       <c r="M8" t="n">
-        <v>0.910683705181684</v>
+        <v>0.590574705571311</v>
       </c>
       <c r="N8" t="n">
-        <v>0.910683705181684</v>
+        <v>0.703065125680132</v>
       </c>
     </row>
     <row r="9">
@@ -975,37 +981,37 @@
         <v>34</v>
       </c>
       <c r="D9" t="n">
-        <v>0.0113685945971</v>
+        <v>0.0224921026264</v>
       </c>
       <c r="E9" t="n">
-        <v>-0.0212840979099</v>
+        <v>-0.01642669564</v>
       </c>
       <c r="F9" t="n">
-        <v>0.0243515154304</v>
+        <v>0.0281163120096</v>
       </c>
       <c r="G9" t="n">
-        <v>-1.87218373635</v>
+        <v>-0.730331704106</v>
       </c>
       <c r="H9" t="n">
-        <v>2.14199875124</v>
+        <v>1.25005262855</v>
       </c>
       <c r="I9" t="n">
-        <v>0.185412662623881</v>
+        <v>0.176310648828552</v>
       </c>
       <c r="J9" t="n">
-        <v>-0.00000000729321027458</v>
+        <v>-0.00000000417124086748</v>
       </c>
       <c r="K9" t="n">
-        <v>0.00000000590121810634</v>
+        <v>0.00000000346760392851</v>
       </c>
       <c r="L9" t="n">
-        <v>-1.23588217604</v>
+        <v>-1.2029173324</v>
       </c>
       <c r="M9" t="n">
-        <v>0.216502363284875</v>
+        <v>0.229008312415435</v>
       </c>
       <c r="N9" t="n">
-        <v>0.560334996103109</v>
+        <v>0.520473437307806</v>
       </c>
     </row>
     <row r="10">
@@ -1019,37 +1025,37 @@
         <v>35</v>
       </c>
       <c r="D10" t="n">
-        <v>0.0111318956599</v>
+        <v>0.0226034903615</v>
       </c>
       <c r="E10" t="n">
-        <v>0.00649428781169</v>
+        <v>0.0124601720723</v>
       </c>
       <c r="F10" t="n">
-        <v>0.00684249483682</v>
+        <v>0.01051525278</v>
       </c>
       <c r="G10" t="n">
-        <v>0.583394599636</v>
+        <v>0.551249911982</v>
       </c>
       <c r="H10" t="n">
-        <v>0.614674719013</v>
+        <v>0.465204825088</v>
       </c>
       <c r="I10" t="n">
-        <v>0.500547330686165</v>
+        <v>0.331001235490514</v>
       </c>
       <c r="J10" t="n">
-        <v>-0.00000000149555633</v>
+        <v>-0.00000000150216536122</v>
       </c>
       <c r="K10" t="n">
-        <v>0.00000000176865901165</v>
+        <v>0.00000000133694403452</v>
       </c>
       <c r="L10" t="n">
-        <v>-0.84558771371</v>
+        <v>-1.12358133357</v>
       </c>
       <c r="M10" t="n">
-        <v>0.397782781925568</v>
+        <v>0.261190678625614</v>
       </c>
       <c r="N10" t="n">
-        <v>0.660536154881473</v>
+        <v>0.544147247136696</v>
       </c>
     </row>
     <row r="11">
@@ -1063,37 +1069,37 @@
         <v>36</v>
       </c>
       <c r="D11" t="n">
-        <v>0.0091354718101</v>
+        <v>0.0185626654146</v>
       </c>
       <c r="E11" t="n">
-        <v>-0.00698254583635</v>
+        <v>-0.0139473346901</v>
       </c>
       <c r="F11" t="n">
-        <v>0.0104115983706</v>
+        <v>0.0160274344277</v>
       </c>
       <c r="G11" t="n">
-        <v>-0.764333356995</v>
+        <v>-0.751364870216</v>
       </c>
       <c r="H11" t="n">
-        <v>1.13968917939</v>
+        <v>0.863423116767</v>
       </c>
       <c r="I11" t="n">
-        <v>0.121840005509611</v>
+        <v>0.0409611913667126</v>
       </c>
       <c r="J11" t="n">
-        <v>-0.00000000357689877979</v>
+        <v>-0.00000000396891093314</v>
       </c>
       <c r="K11" t="n">
-        <v>0.00000000340028042235</v>
+        <v>0.00000000256578684077</v>
       </c>
       <c r="L11" t="n">
-        <v>-1.05194229166</v>
+        <v>-1.54685918178</v>
       </c>
       <c r="M11" t="n">
-        <v>0.292826026955575</v>
+        <v>0.121897205632511</v>
       </c>
       <c r="N11" t="n">
-        <v>0.560334996103109</v>
+        <v>0.405512845618418</v>
       </c>
     </row>
     <row r="12">
@@ -1107,37 +1113,37 @@
         <v>32</v>
       </c>
       <c r="D12" t="n">
-        <v>0.0158392017391</v>
+        <v>0.0245074825214</v>
       </c>
       <c r="E12" t="n">
-        <v>-0.00735995181753</v>
+        <v>-0.00869252444926</v>
       </c>
       <c r="F12" t="n">
-        <v>0.00485251854032</v>
+        <v>0.00698179808053</v>
       </c>
       <c r="G12" t="n">
-        <v>-0.464666839829</v>
+        <v>-0.354688591195</v>
       </c>
       <c r="H12" t="n">
-        <v>0.306361306601</v>
+        <v>0.284884343972</v>
       </c>
       <c r="I12" t="n">
-        <v>0.000000382613149869517</v>
+        <v>0.000000562673325848059</v>
       </c>
       <c r="J12" t="n">
-        <v>-0.00000000212125136724</v>
+        <v>-0.00000000219737209862</v>
       </c>
       <c r="K12" t="n">
-        <v>0.00000000070783657823</v>
+        <v>0.000000000719681658274</v>
       </c>
       <c r="L12" t="n">
-        <v>-2.99680947903</v>
+        <v>-3.05325566291</v>
       </c>
       <c r="M12" t="n">
-        <v>0.00272821159936071</v>
+        <v>0.00226372985852863</v>
       </c>
       <c r="N12" t="n">
-        <v>0.0409231739904107</v>
+        <v>0.0230339501796225</v>
       </c>
     </row>
     <row r="13">
@@ -1151,37 +1157,37 @@
         <v>33</v>
       </c>
       <c r="D13" t="n">
-        <v>0.0170143087946</v>
+        <v>0.0249590725562</v>
       </c>
       <c r="E13" t="n">
-        <v>0.0115885684388</v>
+        <v>0.0163729298561</v>
       </c>
       <c r="F13" t="n">
-        <v>0.0142802161307</v>
+        <v>0.0171925912148</v>
       </c>
       <c r="G13" t="n">
-        <v>0.681107212677</v>
+        <v>0.655991115824</v>
       </c>
       <c r="H13" t="n">
-        <v>0.839306274679</v>
+        <v>0.688831332819</v>
       </c>
       <c r="I13" t="n">
-        <v>0.704635420890283</v>
+        <v>0.618639966531024</v>
       </c>
       <c r="J13" t="n">
-        <v>-0.00000000124476254202</v>
+        <v>-0.00000000128712224349</v>
       </c>
       <c r="K13" t="n">
-        <v>0.00000000231367042723</v>
+        <v>0.00000000192526303903</v>
       </c>
       <c r="L13" t="n">
-        <v>-0.538003393817</v>
+        <v>-0.668543579445</v>
       </c>
       <c r="M13" t="n">
-        <v>0.590574705571311</v>
+        <v>0.503786673631898</v>
       </c>
       <c r="N13" t="n">
-        <v>0.681432352582282</v>
+        <v>0.638832663452972</v>
       </c>
     </row>
     <row r="14">
@@ -1195,37 +1201,37 @@
         <v>34</v>
       </c>
       <c r="D14" t="n">
-        <v>0.0224921026264</v>
+        <v>0.0335382767009</v>
       </c>
       <c r="E14" t="n">
-        <v>-0.01642669564</v>
+        <v>0.00144178399706</v>
       </c>
       <c r="F14" t="n">
-        <v>0.0281163120096</v>
+        <v>0.0304393780382</v>
       </c>
       <c r="G14" t="n">
-        <v>-0.730331704106</v>
+        <v>0.0429892093119</v>
       </c>
       <c r="H14" t="n">
-        <v>1.25005262855</v>
+        <v>0.907601136148</v>
       </c>
       <c r="I14" t="n">
-        <v>0.176310648828552</v>
+        <v>0.303498232820753</v>
       </c>
       <c r="J14" t="n">
-        <v>-0.00000000417124086748</v>
+        <v>-0.00000000216094968249</v>
       </c>
       <c r="K14" t="n">
-        <v>0.00000000346760392851</v>
+        <v>0.0000000025604361311</v>
       </c>
       <c r="L14" t="n">
-        <v>-1.2029173324</v>
+        <v>-0.843977186639</v>
       </c>
       <c r="M14" t="n">
-        <v>0.229008312415435</v>
+        <v>0.398682153887845</v>
       </c>
       <c r="N14" t="n">
-        <v>0.560334996103109</v>
+        <v>0.63497534077209</v>
       </c>
     </row>
     <row r="15">
@@ -1239,37 +1245,37 @@
         <v>35</v>
       </c>
       <c r="D15" t="n">
-        <v>0.0226034903615</v>
+        <v>0.0336612393664</v>
       </c>
       <c r="E15" t="n">
-        <v>0.0124601720723</v>
+        <v>0.0412777362696</v>
       </c>
       <c r="F15" t="n">
-        <v>0.01051525278</v>
+        <v>0.0167484043312</v>
       </c>
       <c r="G15" t="n">
-        <v>0.551249911982</v>
+        <v>1.22626905743</v>
       </c>
       <c r="H15" t="n">
-        <v>0.465204825088</v>
+        <v>0.497557566106</v>
       </c>
       <c r="I15" t="n">
-        <v>0.331001235490514</v>
+        <v>0.650283003861306</v>
       </c>
       <c r="J15" t="n">
-        <v>-0.00000000150216536122</v>
+        <v>0.000000000201236141568</v>
       </c>
       <c r="K15" t="n">
-        <v>0.00000000133694403452</v>
+        <v>0.00000000124250666193</v>
       </c>
       <c r="L15" t="n">
-        <v>-1.12358133357</v>
+        <v>0.161959808937</v>
       </c>
       <c r="M15" t="n">
-        <v>0.261190678625614</v>
+        <v>0.871337503756211</v>
       </c>
       <c r="N15" t="n">
-        <v>0.560334996103109</v>
+        <v>0.907643233079387</v>
       </c>
     </row>
     <row r="16">
@@ -1283,1357 +1289,2677 @@
         <v>36</v>
       </c>
       <c r="D16" t="n">
-        <v>0.0185626654146</v>
+        <v>0.0279980788971</v>
       </c>
       <c r="E16" t="n">
-        <v>-0.0139473346901</v>
+        <v>-0.0109875650233</v>
       </c>
       <c r="F16" t="n">
-        <v>0.0160274344277</v>
+        <v>0.0192801894087</v>
       </c>
       <c r="G16" t="n">
-        <v>-0.751364870216</v>
+        <v>-0.392439962175</v>
       </c>
       <c r="H16" t="n">
-        <v>0.863423116767</v>
+        <v>0.688625440323</v>
       </c>
       <c r="I16" t="n">
-        <v>0.0409611913667126</v>
+        <v>0.043170307228009</v>
       </c>
       <c r="J16" t="n">
-        <v>-0.00000000396891093314</v>
+        <v>-0.0000000032553315556</v>
       </c>
       <c r="K16" t="n">
-        <v>0.00000000256578684077</v>
+        <v>0.00000000214868725155</v>
       </c>
       <c r="L16" t="n">
-        <v>-1.54685918178</v>
+        <v>-1.51503275</v>
       </c>
       <c r="M16" t="n">
-        <v>0.121897205632511</v>
+        <v>0.129764110597894</v>
       </c>
       <c r="N16" t="n">
-        <v>0.560334996103109</v>
+        <v>0.405512845618418</v>
       </c>
     </row>
     <row r="17">
       <c r="A17" t="s">
+        <v>30</v>
+      </c>
+      <c r="B17" t="s">
         <v>39</v>
-      </c>
-      <c r="B17" t="s">
-        <v>31</v>
       </c>
       <c r="C17" t="s">
         <v>32</v>
       </c>
       <c r="D17" t="n">
-        <v>0.00365113562648</v>
+        <v>0.0330351866139</v>
       </c>
       <c r="E17" t="n">
-        <v>-0.00490787906877</v>
+        <v>-0.0100766934353</v>
       </c>
       <c r="F17" t="n">
-        <v>0.0022770713991</v>
+        <v>0.00966581119077</v>
       </c>
       <c r="G17" t="n">
-        <v>-1.3442061788</v>
+        <v>-0.305029105878</v>
       </c>
       <c r="H17" t="n">
-        <v>0.623661137809</v>
+        <v>0.292591390621</v>
       </c>
       <c r="I17" t="n">
-        <v>0.0000436655858588714</v>
+        <v>0.00000297284822221552</v>
       </c>
       <c r="J17" t="n">
-        <v>-0.0000000174282791656</v>
+        <v>-0.00000000223703530663</v>
       </c>
       <c r="K17" t="n">
-        <v>0.00000000612944552773</v>
+        <v>0.000000000747465907153</v>
       </c>
       <c r="L17" t="n">
-        <v>-2.84336961422</v>
+        <v>-2.99282587369</v>
       </c>
       <c r="M17" t="n">
-        <v>0.00446392697220307</v>
+        <v>0.0027640740215547</v>
       </c>
       <c r="N17" t="n">
-        <v>0.066958904583046</v>
+        <v>0.0230339501796225</v>
       </c>
     </row>
     <row r="18">
       <c r="A18" t="s">
+        <v>30</v>
+      </c>
+      <c r="B18" t="s">
         <v>39</v>
-      </c>
-      <c r="B18" t="s">
-        <v>31</v>
       </c>
       <c r="C18" t="s">
         <v>33</v>
       </c>
       <c r="D18" t="n">
-        <v>0.00434177313506</v>
+        <v>0.0325320965269</v>
       </c>
       <c r="E18" t="n">
-        <v>0.00188977712363</v>
+        <v>0.0215104860527</v>
       </c>
       <c r="F18" t="n">
-        <v>0.00787181289508</v>
+        <v>0.0198024070732</v>
       </c>
       <c r="G18" t="n">
-        <v>0.435254690847</v>
+        <v>0.661208109811</v>
       </c>
       <c r="H18" t="n">
-        <v>1.81304104342</v>
+        <v>0.608703686122</v>
       </c>
       <c r="I18" t="n">
-        <v>0.755789174082497</v>
+        <v>0.579366369503906</v>
       </c>
       <c r="J18" t="n">
-        <v>-0.00000001169282982</v>
+        <v>-0.00000000128295535458</v>
       </c>
       <c r="K18" t="n">
-        <v>0.00000001932076661</v>
+        <v>0.00000000173222250637</v>
       </c>
       <c r="L18" t="n">
-        <v>-0.605194920889</v>
+        <v>-0.740641199302</v>
       </c>
       <c r="M18" t="n">
-        <v>0.545049490213788</v>
+        <v>0.458911020651149</v>
       </c>
       <c r="N18" t="n">
-        <v>0.783680463786123</v>
+        <v>0.638832663452972</v>
       </c>
     </row>
     <row r="19">
       <c r="A19" t="s">
+        <v>30</v>
+      </c>
+      <c r="B19" t="s">
         <v>39</v>
-      </c>
-      <c r="B19" t="s">
-        <v>31</v>
       </c>
       <c r="C19" t="s">
         <v>34</v>
       </c>
       <c r="D19" t="n">
-        <v>0.00566886405815</v>
+        <v>0.0445886445908</v>
       </c>
       <c r="E19" t="n">
-        <v>0.0675052645478</v>
+        <v>0.0227482479388</v>
       </c>
       <c r="F19" t="n">
-        <v>0.0262023003402</v>
+        <v>0.0318973117277</v>
       </c>
       <c r="G19" t="n">
-        <v>11.9080760899</v>
+        <v>0.51018029697</v>
       </c>
       <c r="H19" t="n">
-        <v>4.6221430028</v>
+        <v>0.715368498424</v>
       </c>
       <c r="I19" t="n">
-        <v>0.0105549222030537</v>
+        <v>0.501528599462591</v>
       </c>
       <c r="J19" t="n">
-        <v>0.000000117928895427</v>
+        <v>-0.000000000896968259326</v>
       </c>
       <c r="K19" t="n">
-        <v>0.0000000452085165753</v>
+        <v>0.00000000205323678105</v>
       </c>
       <c r="L19" t="n">
-        <v>2.6085548556</v>
+        <v>-0.436855733154</v>
       </c>
       <c r="M19" t="n">
-        <v>0.00909254369830249</v>
+        <v>0.662215976995493</v>
       </c>
       <c r="N19" t="n">
-        <v>0.0681940777372687</v>
+        <v>0.752518155676696</v>
       </c>
     </row>
     <row r="20">
       <c r="A20" t="s">
+        <v>30</v>
+      </c>
+      <c r="B20" t="s">
         <v>39</v>
-      </c>
-      <c r="B20" t="s">
-        <v>31</v>
       </c>
       <c r="C20" t="s">
         <v>35</v>
       </c>
       <c r="D20" t="n">
-        <v>0.00551050559128</v>
+        <v>0.0446037423259</v>
       </c>
       <c r="E20" t="n">
-        <v>0.00696871813282</v>
+        <v>0.0686153831102</v>
       </c>
       <c r="F20" t="n">
-        <v>0.00860104499114</v>
+        <v>0.0288450929469</v>
       </c>
       <c r="G20" t="n">
-        <v>1.26462409254</v>
+        <v>1.53833242531</v>
       </c>
       <c r="H20" t="n">
-        <v>1.56084498031</v>
+        <v>0.646696699486</v>
       </c>
       <c r="I20" t="n">
-        <v>0.866999992558721</v>
+        <v>0.405009304068497</v>
       </c>
       <c r="J20" t="n">
-        <v>0.00000000460681031916</v>
+        <v>0.00000000106045453768</v>
       </c>
       <c r="K20" t="n">
-        <v>0.0000000167809648284</v>
+        <v>0.0000000016136475762</v>
       </c>
       <c r="L20" t="n">
-        <v>0.27452595046</v>
+        <v>0.65717852728</v>
       </c>
       <c r="M20" t="n">
-        <v>0.783680463786123</v>
+        <v>0.511066130762377</v>
       </c>
       <c r="N20" t="n">
-        <v>0.783680463786123</v>
+        <v>0.638832663452972</v>
       </c>
     </row>
     <row r="21">
       <c r="A21" t="s">
+        <v>30</v>
+      </c>
+      <c r="B21" t="s">
         <v>39</v>
-      </c>
-      <c r="B21" t="s">
-        <v>31</v>
       </c>
       <c r="C21" t="s">
         <v>36</v>
       </c>
       <c r="D21" t="n">
-        <v>0.00451170653224</v>
+        <v>0.0376213753064</v>
       </c>
       <c r="E21" t="n">
-        <v>0.0228491709541</v>
+        <v>-0.00755408007152</v>
       </c>
       <c r="F21" t="n">
-        <v>0.0119358572806</v>
+        <v>0.0214609850647</v>
       </c>
       <c r="G21" t="n">
-        <v>5.06441870517</v>
+        <v>-0.200792236063</v>
       </c>
       <c r="H21" t="n">
-        <v>2.64553050943</v>
+        <v>0.570446584952</v>
       </c>
       <c r="I21" t="n">
-        <v>0.120817902734948</v>
+        <v>0.0363172348593641</v>
       </c>
       <c r="J21" t="n">
-        <v>0.0000000507757278841</v>
+        <v>-0.00000000289757644643</v>
       </c>
       <c r="K21" t="n">
-        <v>0.000000029438176856</v>
+        <v>0.00000000185405453924</v>
       </c>
       <c r="L21" t="n">
-        <v>1.72482583186</v>
+        <v>-1.56283236825</v>
       </c>
       <c r="M21" t="n">
-        <v>0.0845588649691196</v>
+        <v>0.118092028679317</v>
       </c>
       <c r="N21" t="n">
-        <v>0.140931441615199</v>
+        <v>0.405512845618418</v>
       </c>
     </row>
     <row r="22">
       <c r="A22" t="s">
-        <v>39</v>
+        <v>30</v>
       </c>
       <c r="B22" t="s">
-        <v>37</v>
+        <v>40</v>
       </c>
       <c r="C22" t="s">
         <v>32</v>
       </c>
       <c r="D22" t="n">
-        <v>0.00799609606119</v>
+        <v>0.0415503092603</v>
       </c>
       <c r="E22" t="n">
-        <v>-0.00635861356138</v>
+        <v>-0.0049662258481</v>
       </c>
       <c r="F22" t="n">
-        <v>0.00375204387649</v>
+        <v>0.0107382313372</v>
       </c>
       <c r="G22" t="n">
-        <v>-0.79521475389</v>
+        <v>-0.119523198178</v>
       </c>
       <c r="H22" t="n">
-        <v>0.469234467393</v>
+        <v>0.25843926383</v>
       </c>
       <c r="I22" t="n">
-        <v>0.00000821428740448652</v>
+        <v>0.0000100190192678637</v>
       </c>
       <c r="J22" t="n">
-        <v>-0.0000000111453850315</v>
+        <v>-0.00000000190521958287</v>
       </c>
       <c r="K22" t="n">
-        <v>0.00000000465372964999</v>
+        <v>0.000000000724729743801</v>
       </c>
       <c r="L22" t="n">
-        <v>-2.39493607702</v>
+        <v>-2.6288690359</v>
       </c>
       <c r="M22" t="n">
-        <v>0.0166232630726543</v>
+        <v>0.00856693464450145</v>
       </c>
       <c r="N22" t="n">
-        <v>0.0770253258464087</v>
+        <v>0.0535433415281341</v>
       </c>
     </row>
     <row r="23">
       <c r="A23" t="s">
-        <v>39</v>
+        <v>30</v>
       </c>
       <c r="B23" t="s">
-        <v>37</v>
+        <v>40</v>
       </c>
       <c r="C23" t="s">
         <v>33</v>
       </c>
       <c r="D23" t="n">
-        <v>0.00866542898789</v>
+        <v>0.0396572210203</v>
       </c>
       <c r="E23" t="n">
-        <v>0.00735232765088</v>
+        <v>0.0253611093451</v>
       </c>
       <c r="F23" t="n">
-        <v>0.0128325888609</v>
+        <v>0.0225724572696</v>
       </c>
       <c r="G23" t="n">
-        <v>0.848466666932</v>
+        <v>0.639507980959</v>
       </c>
       <c r="H23" t="n">
-        <v>1.48089481535</v>
+        <v>0.569189083069</v>
       </c>
       <c r="I23" t="n">
-        <v>0.918622620370358</v>
+        <v>0.528693006729337</v>
       </c>
       <c r="J23" t="n">
-        <v>-0.00000000599226165586</v>
+        <v>-0.00000000137820918634</v>
       </c>
       <c r="K23" t="n">
-        <v>0.0000000159723912979</v>
+        <v>0.00000000165994619294</v>
       </c>
       <c r="L23" t="n">
-        <v>-0.375163714944</v>
+        <v>-0.830273410187</v>
       </c>
       <c r="M23" t="n">
-        <v>0.707538713920786</v>
+        <v>0.406384218094138</v>
       </c>
       <c r="N23" t="n">
-        <v>0.783680463786123</v>
+        <v>0.63497534077209</v>
       </c>
     </row>
     <row r="24">
       <c r="A24" t="s">
-        <v>39</v>
+        <v>30</v>
       </c>
       <c r="B24" t="s">
-        <v>37</v>
+        <v>40</v>
       </c>
       <c r="C24" t="s">
         <v>34</v>
       </c>
       <c r="D24" t="n">
-        <v>0.0113685945971</v>
+        <v>0.055623243735</v>
       </c>
       <c r="E24" t="n">
-        <v>0.0769877554691</v>
+        <v>0.0399436969931</v>
       </c>
       <c r="F24" t="n">
-        <v>0.0311107611213</v>
+        <v>0.0343465353481</v>
       </c>
       <c r="G24" t="n">
-        <v>6.77196770554</v>
+        <v>0.718111607864</v>
       </c>
       <c r="H24" t="n">
-        <v>2.73655295345</v>
+        <v>0.617485300061</v>
       </c>
       <c r="I24" t="n">
-        <v>0.0231502423699982</v>
+        <v>0.65249038324923</v>
       </c>
       <c r="J24" t="n">
-        <v>0.0000000620945164504</v>
+        <v>-0.000000000372064993653</v>
       </c>
       <c r="K24" t="n">
-        <v>0.0000000269275097403</v>
+        <v>0.00000000178634068122</v>
       </c>
       <c r="L24" t="n">
-        <v>2.30598807871</v>
+        <v>-0.208283334509</v>
       </c>
       <c r="M24" t="n">
-        <v>0.0211112984661059</v>
+        <v>0.835007743438737</v>
       </c>
       <c r="N24" t="n">
-        <v>0.0770253258464087</v>
+        <v>0.90761711243341</v>
       </c>
     </row>
     <row r="25">
       <c r="A25" t="s">
-        <v>39</v>
+        <v>30</v>
       </c>
       <c r="B25" t="s">
-        <v>37</v>
+        <v>40</v>
       </c>
       <c r="C25" t="s">
         <v>35</v>
       </c>
       <c r="D25" t="n">
-        <v>0.0111318956599</v>
+        <v>0.0555658723413</v>
       </c>
       <c r="E25" t="n">
-        <v>0.012737240389</v>
+        <v>0.0849583930792</v>
       </c>
       <c r="F25" t="n">
-        <v>0.0105445475329</v>
+        <v>0.0320062975787</v>
       </c>
       <c r="G25" t="n">
-        <v>1.14421126268</v>
+        <v>1.52896714295</v>
       </c>
       <c r="H25" t="n">
-        <v>0.947237366844</v>
+        <v>0.576006390796</v>
       </c>
       <c r="I25" t="n">
-        <v>0.880152292348081</v>
+        <v>0.357933504253644</v>
       </c>
       <c r="J25" t="n">
-        <v>0.00000000281826286657</v>
+        <v>0.00000000091621951527</v>
       </c>
       <c r="K25" t="n">
-        <v>0.000000010261355936</v>
+        <v>0.000000001363934808</v>
       </c>
       <c r="L25" t="n">
-        <v>0.274648193099</v>
+        <v>0.671747293123</v>
       </c>
       <c r="M25" t="n">
-        <v>0.78358653681939</v>
+        <v>0.501744588069446</v>
       </c>
       <c r="N25" t="n">
-        <v>0.783680463786123</v>
+        <v>0.638832663452972</v>
       </c>
     </row>
     <row r="26">
       <c r="A26" t="s">
-        <v>39</v>
+        <v>30</v>
       </c>
       <c r="B26" t="s">
-        <v>37</v>
+        <v>40</v>
       </c>
       <c r="C26" t="s">
         <v>36</v>
       </c>
       <c r="D26" t="n">
-        <v>0.0091354718101</v>
+        <v>0.0472146439979</v>
       </c>
       <c r="E26" t="n">
-        <v>0.0374764413795</v>
+        <v>0.00319075268037</v>
       </c>
       <c r="F26" t="n">
-        <v>0.0169600475779</v>
+        <v>0.0229936517586</v>
       </c>
       <c r="G26" t="n">
-        <v>4.1022994935</v>
+        <v>0.0675797254875</v>
       </c>
       <c r="H26" t="n">
-        <v>1.85650483417</v>
+        <v>0.487002544371</v>
       </c>
       <c r="I26" t="n">
-        <v>0.0882085367226271</v>
+        <v>0.0598912725300036</v>
       </c>
       <c r="J26" t="n">
-        <v>0.0000000396885431252</v>
+        <v>-0.00000000221121006163</v>
       </c>
       <c r="K26" t="n">
-        <v>0.0000000211271022446</v>
+        <v>0.00000000167319657136</v>
       </c>
       <c r="L26" t="n">
-        <v>1.87856065947</v>
+        <v>-1.32154828637</v>
       </c>
       <c r="M26" t="n">
-        <v>0.0603045070926175</v>
+        <v>0.186318613378225</v>
       </c>
       <c r="N26" t="n">
-        <v>0.129223943769895</v>
+        <v>0.517551703828402</v>
       </c>
     </row>
     <row r="27">
       <c r="A27" t="s">
-        <v>39</v>
+        <v>41</v>
       </c>
       <c r="B27" t="s">
-        <v>38</v>
+        <v>31</v>
       </c>
       <c r="C27" t="s">
         <v>32</v>
       </c>
       <c r="D27" t="n">
-        <v>0.0158392017391</v>
+        <v>0.00799609606119</v>
       </c>
       <c r="E27" t="n">
-        <v>-0.00919671121886</v>
+        <v>-0.00635861356138</v>
       </c>
       <c r="F27" t="n">
-        <v>0.00705478749554</v>
+        <v>0.00375204387649</v>
       </c>
       <c r="G27" t="n">
-        <v>-0.58062971672</v>
+        <v>-0.79521475389</v>
       </c>
       <c r="H27" t="n">
-        <v>0.445400444526</v>
+        <v>0.469234467393</v>
       </c>
       <c r="I27" t="n">
-        <v>0.0000619170991732805</v>
+        <v>0.00000821428740448652</v>
       </c>
       <c r="J27" t="n">
-        <v>-0.0000000101067701998</v>
+        <v>-0.0000000111453850315</v>
       </c>
       <c r="K27" t="n">
-        <v>0.0000000045299679244</v>
+        <v>0.00000000465372964999</v>
       </c>
       <c r="L27" t="n">
-        <v>-2.23109089698</v>
+        <v>-2.39493607702</v>
       </c>
       <c r="M27" t="n">
-        <v>0.0256751086154696</v>
+        <v>0.0166232630726543</v>
       </c>
       <c r="N27" t="n">
-        <v>0.0770253258464087</v>
+        <v>0.160469428846685</v>
       </c>
     </row>
     <row r="28">
       <c r="A28" t="s">
-        <v>39</v>
+        <v>41</v>
       </c>
       <c r="B28" t="s">
-        <v>38</v>
+        <v>31</v>
       </c>
       <c r="C28" t="s">
         <v>33</v>
       </c>
       <c r="D28" t="n">
-        <v>0.0170143087946</v>
+        <v>0.00866542898789</v>
       </c>
       <c r="E28" t="n">
-        <v>0.0158866014821</v>
+        <v>0.00735232765088</v>
       </c>
       <c r="F28" t="n">
-        <v>0.0199995113064</v>
+        <v>0.0128325888609</v>
       </c>
       <c r="G28" t="n">
-        <v>0.933720063143</v>
+        <v>0.848466666932</v>
       </c>
       <c r="H28" t="n">
-        <v>1.17545247049</v>
+        <v>1.48089481535</v>
       </c>
       <c r="I28" t="n">
-        <v>0.955031761880117</v>
+        <v>0.918622620370358</v>
       </c>
       <c r="J28" t="n">
-        <v>-0.0000000046572993829</v>
+        <v>-0.00000000599226165586</v>
       </c>
       <c r="K28" t="n">
-        <v>0.0000000126447890221</v>
+        <v>0.0000000159723912979</v>
       </c>
       <c r="L28" t="n">
-        <v>-0.36831768207</v>
+        <v>-0.375163714944</v>
       </c>
       <c r="M28" t="n">
-        <v>0.712636369445213</v>
+        <v>0.707538713920786</v>
       </c>
       <c r="N28" t="n">
-        <v>0.783680463786123</v>
+        <v>0.851724496542815</v>
       </c>
     </row>
     <row r="29">
       <c r="A29" t="s">
-        <v>39</v>
+        <v>41</v>
       </c>
       <c r="B29" t="s">
-        <v>38</v>
+        <v>31</v>
       </c>
       <c r="C29" t="s">
         <v>34</v>
       </c>
       <c r="D29" t="n">
-        <v>0.0224921026264</v>
+        <v>0.0113685945971</v>
       </c>
       <c r="E29" t="n">
-        <v>0.0812096147603</v>
+        <v>0.0769877554691</v>
       </c>
       <c r="F29" t="n">
-        <v>0.035533036312</v>
+        <v>0.0311107611213</v>
       </c>
       <c r="G29" t="n">
-        <v>3.6105835061</v>
+        <v>6.77196770554</v>
       </c>
       <c r="H29" t="n">
-        <v>1.57980055944</v>
+        <v>2.73655295345</v>
       </c>
       <c r="I29" t="n">
-        <v>0.0792589622496275</v>
+        <v>0.0231502423699982</v>
       </c>
       <c r="J29" t="n">
-        <v>0.0000000280446241936</v>
+        <v>0.0000000620945164504</v>
       </c>
       <c r="K29" t="n">
-        <v>0.0000000159501483137</v>
+        <v>0.0000000269275097403</v>
       </c>
       <c r="L29" t="n">
-        <v>1.75826729896</v>
+        <v>2.30598807871</v>
       </c>
       <c r="M29" t="n">
-        <v>0.0787020390174739</v>
+        <v>0.0211112984661059</v>
       </c>
       <c r="N29" t="n">
-        <v>0.140931441615199</v>
+        <v>0.160469428846685</v>
       </c>
     </row>
     <row r="30">
       <c r="A30" t="s">
-        <v>39</v>
+        <v>41</v>
       </c>
       <c r="B30" t="s">
-        <v>38</v>
+        <v>31</v>
       </c>
       <c r="C30" t="s">
         <v>35</v>
       </c>
       <c r="D30" t="n">
-        <v>0.0226034903615</v>
+        <v>0.0111318956599</v>
       </c>
       <c r="E30" t="n">
-        <v>0.0179885442573</v>
+        <v>0.012737240389</v>
       </c>
       <c r="F30" t="n">
-        <v>0.0141532971362</v>
+        <v>0.0105445475329</v>
       </c>
       <c r="G30" t="n">
-        <v>0.795830377061</v>
+        <v>1.14421126268</v>
       </c>
       <c r="H30" t="n">
-        <v>0.626155381749</v>
+        <v>0.947237366844</v>
       </c>
       <c r="I30" t="n">
-        <v>0.746882748428176</v>
+        <v>0.880152292348081</v>
       </c>
       <c r="J30" t="n">
-        <v>-0.0000000019489446406</v>
+        <v>0.00000000281826286657</v>
       </c>
       <c r="K30" t="n">
-        <v>0.00000000694539204337</v>
+        <v>0.000000010261355936</v>
       </c>
       <c r="L30" t="n">
-        <v>-0.280609737856</v>
+        <v>0.274648193099</v>
       </c>
       <c r="M30" t="n">
-        <v>0.779009746291693</v>
+        <v>0.78358653681939</v>
       </c>
       <c r="N30" t="n">
-        <v>0.783680463786123</v>
+        <v>0.851724496542815</v>
       </c>
     </row>
     <row r="31">
       <c r="A31" t="s">
-        <v>39</v>
+        <v>41</v>
       </c>
       <c r="B31" t="s">
-        <v>38</v>
+        <v>31</v>
       </c>
       <c r="C31" t="s">
         <v>36</v>
       </c>
       <c r="D31" t="n">
-        <v>0.0185626654146</v>
+        <v>0.0091354718101</v>
       </c>
       <c r="E31" t="n">
-        <v>0.0557638400393</v>
+        <v>0.0374764413795</v>
       </c>
       <c r="F31" t="n">
-        <v>0.0215812822775</v>
+        <v>0.0169600475779</v>
       </c>
       <c r="G31" t="n">
-        <v>3.00408582464</v>
+        <v>4.1022994935</v>
       </c>
       <c r="H31" t="n">
-        <v>1.16261764114</v>
+        <v>1.85650483417</v>
       </c>
       <c r="I31" t="n">
-        <v>0.0777998587536567</v>
+        <v>0.0882085367226271</v>
       </c>
       <c r="J31" t="n">
-        <v>0.0000000288826239131</v>
+        <v>0.0000000396885431252</v>
       </c>
       <c r="K31" t="n">
-        <v>0.0000000141720647192</v>
+        <v>0.0000000211271022446</v>
       </c>
       <c r="L31" t="n">
-        <v>2.03799689639</v>
+        <v>1.87856065947</v>
       </c>
       <c r="M31" t="n">
-        <v>0.0415502432560626</v>
+        <v>0.0603045070926175</v>
       </c>
       <c r="N31" t="n">
-        <v>0.103875608140156</v>
+        <v>0.215373239616491</v>
       </c>
     </row>
     <row r="32">
       <c r="A32" t="s">
-        <v>40</v>
+        <v>41</v>
       </c>
       <c r="B32" t="s">
-        <v>31</v>
+        <v>37</v>
       </c>
       <c r="C32" t="s">
         <v>32</v>
       </c>
       <c r="D32" t="n">
-        <v>0.00365113562648</v>
+        <v>0.0158392017391</v>
       </c>
       <c r="E32" t="n">
-        <v>0.000283149513671</v>
+        <v>-0.00919671121886</v>
       </c>
       <c r="F32" t="n">
-        <v>0.00272803987039</v>
+        <v>0.00705478749554</v>
       </c>
       <c r="G32" t="n">
-        <v>0.077551080715</v>
+        <v>-0.58062971672</v>
       </c>
       <c r="H32" t="n">
-        <v>0.747175714484</v>
+        <v>0.445400444526</v>
       </c>
       <c r="I32" t="n">
-        <v>0.232689794163237</v>
+        <v>0.0000619170991732805</v>
       </c>
       <c r="J32" t="n">
-        <v>-0.000000000905719748124</v>
+        <v>-0.0000000101067701998</v>
       </c>
       <c r="K32" t="n">
-        <v>0.00000000214666548724</v>
+        <v>0.0000000045299679244</v>
       </c>
       <c r="L32" t="n">
-        <v>-0.421919369137</v>
+        <v>-2.23109089698</v>
       </c>
       <c r="M32" t="n">
-        <v>0.673083871763834</v>
+        <v>0.0256751086154696</v>
       </c>
       <c r="N32" t="n">
-        <v>0.841354839704793</v>
+        <v>0.160469428846685</v>
       </c>
     </row>
     <row r="33">
       <c r="A33" t="s">
-        <v>40</v>
+        <v>41</v>
       </c>
       <c r="B33" t="s">
-        <v>31</v>
+        <v>37</v>
       </c>
       <c r="C33" t="s">
         <v>33</v>
       </c>
       <c r="D33" t="n">
-        <v>0.00434177313506</v>
+        <v>0.0170143087946</v>
       </c>
       <c r="E33" t="n">
-        <v>0.00105471304044</v>
+        <v>0.0158866014821</v>
       </c>
       <c r="F33" t="n">
-        <v>0.00727029122102</v>
+        <v>0.0199995113064</v>
       </c>
       <c r="G33" t="n">
-        <v>0.242922190459</v>
+        <v>0.933720063143</v>
       </c>
       <c r="H33" t="n">
-        <v>1.67449818193</v>
+        <v>1.17545247049</v>
       </c>
       <c r="I33" t="n">
-        <v>0.652937139007057</v>
+        <v>0.955031761880117</v>
       </c>
       <c r="J33" t="n">
-        <v>-0.00000000280491224162</v>
+        <v>-0.0000000046572993829</v>
       </c>
       <c r="K33" t="n">
-        <v>0.00000000482131184025</v>
+        <v>0.0000000126447890221</v>
       </c>
       <c r="L33" t="n">
-        <v>-0.58177366131</v>
+        <v>-0.36831768207</v>
       </c>
       <c r="M33" t="n">
-        <v>0.560719147392072</v>
+        <v>0.712636369445213</v>
       </c>
       <c r="N33" t="n">
-        <v>0.764617019171007</v>
+        <v>0.851724496542815</v>
       </c>
     </row>
     <row r="34">
       <c r="A34" t="s">
-        <v>40</v>
+        <v>41</v>
       </c>
       <c r="B34" t="s">
-        <v>31</v>
+        <v>37</v>
       </c>
       <c r="C34" t="s">
         <v>34</v>
       </c>
       <c r="D34" t="n">
-        <v>0.00566886405815</v>
+        <v>0.0224921026264</v>
       </c>
       <c r="E34" t="n">
-        <v>-0.015819062407</v>
+        <v>0.0812096147603</v>
       </c>
       <c r="F34" t="n">
-        <v>0.0235470726045</v>
+        <v>0.035533036312</v>
       </c>
       <c r="G34" t="n">
-        <v>-2.79051715559</v>
+        <v>3.6105835061</v>
       </c>
       <c r="H34" t="n">
-        <v>4.15375503152</v>
+        <v>1.57980055944</v>
       </c>
       <c r="I34" t="n">
-        <v>0.346416558133099</v>
+        <v>0.0792589622496275</v>
       </c>
       <c r="J34" t="n">
-        <v>-0.0000000112854646676</v>
+        <v>0.0000000280446241936</v>
       </c>
       <c r="K34" t="n">
-        <v>0.000000011439937454</v>
+        <v>0.0000000159501483137</v>
       </c>
       <c r="L34" t="n">
-        <v>-0.986497060229</v>
+        <v>1.75826729896</v>
       </c>
       <c r="M34" t="n">
-        <v>0.323889257130468</v>
+        <v>0.0787020390174739</v>
       </c>
       <c r="N34" t="n">
-        <v>0.558210385590131</v>
+        <v>0.218616775048539</v>
       </c>
     </row>
     <row r="35">
       <c r="A35" t="s">
-        <v>40</v>
+        <v>41</v>
       </c>
       <c r="B35" t="s">
-        <v>31</v>
+        <v>37</v>
       </c>
       <c r="C35" t="s">
         <v>35</v>
       </c>
       <c r="D35" t="n">
-        <v>0.00551050559128</v>
+        <v>0.0226034903615</v>
       </c>
       <c r="E35" t="n">
-        <v>-0.0034563339711</v>
+        <v>0.0179885442573</v>
       </c>
       <c r="F35" t="n">
-        <v>0.00346798046263</v>
+        <v>0.0141532971362</v>
       </c>
       <c r="G35" t="n">
-        <v>-0.627226288741</v>
+        <v>0.795830377061</v>
       </c>
       <c r="H35" t="n">
-        <v>0.62933979563</v>
+        <v>0.626155381749</v>
       </c>
       <c r="I35" t="n">
-        <v>0.00974011041317592</v>
+        <v>0.746882748428176</v>
       </c>
       <c r="J35" t="n">
-        <v>-0.00000000454302037444</v>
+        <v>-0.0000000019489446406</v>
       </c>
       <c r="K35" t="n">
-        <v>0.00000000180363674477</v>
+        <v>0.00000000694539204337</v>
       </c>
       <c r="L35" t="n">
-        <v>-2.51881116728</v>
+        <v>-0.280609737856</v>
       </c>
       <c r="M35" t="n">
-        <v>0.0117751787750913</v>
+        <v>0.779009746291693</v>
       </c>
       <c r="N35" t="n">
-        <v>0.0441569204065925</v>
+        <v>0.851724496542815</v>
       </c>
     </row>
     <row r="36">
       <c r="A36" t="s">
-        <v>40</v>
+        <v>41</v>
       </c>
       <c r="B36" t="s">
-        <v>31</v>
+        <v>37</v>
       </c>
       <c r="C36" t="s">
         <v>36</v>
       </c>
       <c r="D36" t="n">
-        <v>0.00451170653224</v>
+        <v>0.0185626654146</v>
       </c>
       <c r="E36" t="n">
-        <v>-0.0114791459085</v>
+        <v>0.0557638400393</v>
       </c>
       <c r="F36" t="n">
-        <v>0.00722535136329</v>
+        <v>0.0215812822775</v>
       </c>
       <c r="G36" t="n">
-        <v>-2.54430243334</v>
+        <v>3.00408582464</v>
       </c>
       <c r="H36" t="n">
-        <v>1.60146749609</v>
+        <v>1.16261764114</v>
       </c>
       <c r="I36" t="n">
-        <v>0.0133624956931359</v>
+        <v>0.0777998587536567</v>
       </c>
       <c r="J36" t="n">
-        <v>-0.0000000109686278534</v>
+        <v>0.0000000288826239131</v>
       </c>
       <c r="K36" t="n">
-        <v>0.00000000419534696223</v>
+        <v>0.0000000141720647192</v>
       </c>
       <c r="L36" t="n">
-        <v>-2.61447454815</v>
+        <v>2.03799689639</v>
       </c>
       <c r="M36" t="n">
-        <v>0.00893648184587932</v>
+        <v>0.0415502432560626</v>
       </c>
       <c r="N36" t="n">
-        <v>0.0441569204065925</v>
+        <v>0.207751216280313</v>
       </c>
     </row>
     <row r="37">
       <c r="A37" t="s">
-        <v>40</v>
+        <v>41</v>
       </c>
       <c r="B37" t="s">
-        <v>37</v>
+        <v>38</v>
       </c>
       <c r="C37" t="s">
         <v>32</v>
       </c>
       <c r="D37" t="n">
-        <v>0.00799609606119</v>
+        <v>0.0245074825214</v>
       </c>
       <c r="E37" t="n">
-        <v>0.00222932693111</v>
+        <v>-0.0114809752054</v>
       </c>
       <c r="F37" t="n">
-        <v>0.00339332996283</v>
+        <v>0.00925429738627</v>
       </c>
       <c r="G37" t="n">
-        <v>0.278801919593</v>
+        <v>-0.468468158465</v>
       </c>
       <c r="H37" t="n">
-        <v>0.424373336296</v>
+        <v>0.377611098087</v>
       </c>
       <c r="I37" t="n">
-        <v>0.105506003223572</v>
+        <v>0.00000991234639999672</v>
       </c>
       <c r="J37" t="n">
-        <v>-0.000000000353836915763</v>
+        <v>-0.0000000101368087815</v>
       </c>
       <c r="K37" t="n">
-        <v>0.00000000122853145732</v>
+        <v>0.00000000406768672937</v>
       </c>
       <c r="L37" t="n">
-        <v>-0.28801616243</v>
+        <v>-2.49203280783</v>
       </c>
       <c r="M37" t="n">
-        <v>0.773334366817085</v>
+        <v>0.0127014304618577</v>
       </c>
       <c r="N37" t="n">
-        <v>0.892308884788944</v>
+        <v>0.160469428846685</v>
       </c>
     </row>
     <row r="38">
       <c r="A38" t="s">
-        <v>40</v>
+        <v>41</v>
       </c>
       <c r="B38" t="s">
-        <v>37</v>
+        <v>38</v>
       </c>
       <c r="C38" t="s">
         <v>33</v>
       </c>
       <c r="D38" t="n">
-        <v>0.00866542898789</v>
+        <v>0.0249590725562</v>
       </c>
       <c r="E38" t="n">
-        <v>0.00463747352943</v>
+        <v>0.0247122083369</v>
       </c>
       <c r="F38" t="n">
-        <v>0.00981363042167</v>
+        <v>0.0259421789167</v>
       </c>
       <c r="G38" t="n">
-        <v>0.535169526623</v>
+        <v>0.990109239084</v>
       </c>
       <c r="H38" t="n">
-        <v>1.13250370355</v>
+        <v>1.03938873763</v>
       </c>
       <c r="I38" t="n">
-        <v>0.681186295423847</v>
+        <v>0.992401045400186</v>
       </c>
       <c r="J38" t="n">
-        <v>-0.00000000195003974656</v>
+        <v>-0.00000000338187130191</v>
       </c>
       <c r="K38" t="n">
-        <v>0.00000000325972714089</v>
+        <v>0.0000000112287350265</v>
       </c>
       <c r="L38" t="n">
-        <v>-0.598221772031</v>
+        <v>-0.301180078961</v>
       </c>
       <c r="M38" t="n">
-        <v>0.54969196593028</v>
+        <v>0.763277179672784</v>
       </c>
       <c r="N38" t="n">
-        <v>0.764617019171007</v>
+        <v>0.851724496542815</v>
       </c>
     </row>
     <row r="39">
       <c r="A39" t="s">
-        <v>40</v>
+        <v>41</v>
       </c>
       <c r="B39" t="s">
-        <v>37</v>
+        <v>38</v>
       </c>
       <c r="C39" t="s">
         <v>34</v>
       </c>
       <c r="D39" t="n">
-        <v>0.0113685945971</v>
+        <v>0.0335382767009</v>
       </c>
       <c r="E39" t="n">
-        <v>-0.0115931743094</v>
+        <v>0.0808032698059</v>
       </c>
       <c r="F39" t="n">
-        <v>0.0259534122571</v>
+        <v>0.0385842351181</v>
       </c>
       <c r="G39" t="n">
-        <v>-1.01975439535</v>
+        <v>2.40928508422</v>
       </c>
       <c r="H39" t="n">
-        <v>2.28290419149</v>
+        <v>1.15045371777</v>
       </c>
       <c r="I39" t="n">
-        <v>0.364636694422173</v>
+        <v>0.201670999606624</v>
       </c>
       <c r="J39" t="n">
-        <v>-0.00000000615026895169</v>
+        <v>0.0000000151299210961</v>
       </c>
       <c r="K39" t="n">
-        <v>0.00000000637836721396</v>
+        <v>0.0000000120168080707</v>
       </c>
       <c r="L39" t="n">
-        <v>-0.964238769168</v>
+        <v>1.2590632227</v>
       </c>
       <c r="M39" t="n">
-        <v>0.334926231354079</v>
+        <v>0.208007496933323</v>
       </c>
       <c r="N39" t="n">
-        <v>0.558210385590131</v>
+        <v>0.472744311212097</v>
       </c>
     </row>
     <row r="40">
       <c r="A40" t="s">
-        <v>40</v>
+        <v>41</v>
       </c>
       <c r="B40" t="s">
-        <v>37</v>
+        <v>38</v>
       </c>
       <c r="C40" t="s">
         <v>35</v>
       </c>
       <c r="D40" t="n">
-        <v>0.0111318956599</v>
+        <v>0.0336612393664</v>
       </c>
       <c r="E40" t="n">
-        <v>-0.000468572351367</v>
+        <v>0.0381908840292</v>
       </c>
       <c r="F40" t="n">
-        <v>0.0053618130074</v>
+        <v>0.0173511838148</v>
       </c>
       <c r="G40" t="n">
-        <v>-0.0420927724875</v>
+        <v>1.13456559378</v>
       </c>
       <c r="H40" t="n">
-        <v>0.48166216889</v>
+        <v>0.51546479397</v>
       </c>
       <c r="I40" t="n">
-        <v>0.025650039091221</v>
+        <v>0.794722805885089</v>
       </c>
       <c r="J40" t="n">
-        <v>-0.00000000297599351093</v>
+        <v>0.00000000267525435864</v>
       </c>
       <c r="K40" t="n">
-        <v>0.00000000134313478436</v>
+        <v>0.00000000575717529108</v>
       </c>
       <c r="L40" t="n">
-        <v>-2.21570727344</v>
+        <v>0.46468176204</v>
       </c>
       <c r="M40" t="n">
-        <v>0.0267115564499915</v>
+        <v>0.642159370859018</v>
       </c>
       <c r="N40" t="n">
-        <v>0.0801346693499745</v>
+        <v>0.851724496542815</v>
       </c>
     </row>
     <row r="41">
       <c r="A41" t="s">
-        <v>40</v>
+        <v>41</v>
       </c>
       <c r="B41" t="s">
-        <v>37</v>
+        <v>38</v>
       </c>
       <c r="C41" t="s">
         <v>36</v>
       </c>
       <c r="D41" t="n">
-        <v>0.0091354718101</v>
+        <v>0.0279980788971</v>
       </c>
       <c r="E41" t="n">
-        <v>-0.0228530866343</v>
+        <v>0.0624639937102</v>
       </c>
       <c r="F41" t="n">
-        <v>0.0119125282179</v>
+        <v>0.0260604005663</v>
       </c>
       <c r="G41" t="n">
-        <v>-2.50157705145</v>
+        <v>2.23100998964</v>
       </c>
       <c r="H41" t="n">
-        <v>1.30398609568</v>
+        <v>0.930792454084</v>
       </c>
       <c r="I41" t="n">
-        <v>0.00273008378634463</v>
+        <v>0.179145196295074</v>
       </c>
       <c r="J41" t="n">
-        <v>-0.0000000111968500215</v>
+        <v>0.0000000187500202691</v>
       </c>
       <c r="K41" t="n">
-        <v>0.00000000350202355095</v>
+        <v>0.0000000120008517836</v>
       </c>
       <c r="L41" t="n">
-        <v>-3.19725149149</v>
+        <v>1.56239078751</v>
       </c>
       <c r="M41" t="n">
-        <v>0.00138743903434683</v>
+        <v>0.118195956026193</v>
       </c>
       <c r="N41" t="n">
-        <v>0.0208115855152025</v>
+        <v>0.295489890065483</v>
       </c>
     </row>
     <row r="42">
       <c r="A42" t="s">
-        <v>40</v>
+        <v>41</v>
       </c>
       <c r="B42" t="s">
-        <v>38</v>
+        <v>39</v>
       </c>
       <c r="C42" t="s">
         <v>32</v>
       </c>
       <c r="D42" t="n">
-        <v>0.0158392017391</v>
+        <v>0.0330351866139</v>
       </c>
       <c r="E42" t="n">
-        <v>0.00910884541401</v>
+        <v>0.00334633678243</v>
       </c>
       <c r="F42" t="n">
-        <v>0.00590761807635</v>
+        <v>0.0192521189814</v>
       </c>
       <c r="G42" t="n">
-        <v>0.57508235352</v>
+        <v>0.101296136799</v>
       </c>
       <c r="H42" t="n">
-        <v>0.372974482783</v>
+        <v>0.58277615339</v>
       </c>
       <c r="I42" t="n">
-        <v>0.265817083546758</v>
+        <v>0.1175222308576</v>
       </c>
       <c r="J42" t="n">
-        <v>0.00000000021986460267</v>
+        <v>-0.00000000375592425671</v>
       </c>
       <c r="K42" t="n">
-        <v>0.00000000112813483351</v>
+        <v>0.00000000662388010093</v>
       </c>
       <c r="L42" t="n">
-        <v>0.194892131809</v>
+        <v>-0.567027814435</v>
       </c>
       <c r="M42" t="n">
-        <v>0.84547739399404</v>
+        <v>0.570695284460423</v>
       </c>
       <c r="N42" t="n">
-        <v>0.905868636422185</v>
+        <v>0.851724496542815</v>
       </c>
     </row>
     <row r="43">
       <c r="A43" t="s">
-        <v>40</v>
+        <v>41</v>
       </c>
       <c r="B43" t="s">
-        <v>38</v>
+        <v>39</v>
       </c>
       <c r="C43" t="s">
         <v>33</v>
       </c>
       <c r="D43" t="n">
-        <v>0.0170143087946</v>
+        <v>0.0325320965269</v>
       </c>
       <c r="E43" t="n">
-        <v>0.0189647884069</v>
+        <v>0.037505134513</v>
       </c>
       <c r="F43" t="n">
-        <v>0.0150771954148</v>
+        <v>0.0315006819938</v>
       </c>
       <c r="G43" t="n">
-        <v>1.11463760508</v>
+        <v>1.15286558559</v>
       </c>
       <c r="H43" t="n">
-        <v>0.886147982667</v>
+        <v>0.968295479136</v>
       </c>
       <c r="I43" t="n">
-        <v>0.896507651971053</v>
+        <v>0.874131670281754</v>
       </c>
       <c r="J43" t="n">
-        <v>-0.000000000219238920646</v>
+        <v>-0.00000000111830975515</v>
       </c>
       <c r="K43" t="n">
-        <v>0.00000000255838368877</v>
+        <v>0.0000000104690981533</v>
       </c>
       <c r="L43" t="n">
-        <v>-0.0856943083277</v>
+        <v>-0.106820065948</v>
       </c>
       <c r="M43" t="n">
-        <v>0.931709426782296</v>
+        <v>0.91493172823201</v>
       </c>
       <c r="N43" t="n">
-        <v>0.931709426782296</v>
+        <v>0.95305388357501</v>
       </c>
     </row>
     <row r="44">
       <c r="A44" t="s">
-        <v>40</v>
+        <v>41</v>
       </c>
       <c r="B44" t="s">
-        <v>38</v>
+        <v>39</v>
       </c>
       <c r="C44" t="s">
         <v>34</v>
       </c>
       <c r="D44" t="n">
-        <v>0.0224921026264</v>
+        <v>0.0445886445908</v>
       </c>
       <c r="E44" t="n">
-        <v>-0.0116710750391</v>
+        <v>0.0873635606304</v>
       </c>
       <c r="F44" t="n">
-        <v>0.031391513915</v>
+        <v>0.0434207337254</v>
       </c>
       <c r="G44" t="n">
-        <v>-0.518896575965</v>
+        <v>1.95932308399</v>
       </c>
       <c r="H44" t="n">
-        <v>1.39566826795</v>
+        <v>0.973806988839</v>
       </c>
       <c r="I44" t="n">
-        <v>0.265776393859218</v>
+        <v>0.308041276931647</v>
       </c>
       <c r="J44" t="n">
-        <v>-0.00000000477036137637</v>
+        <v>0.0000000103370170316</v>
       </c>
       <c r="K44" t="n">
-        <v>0.00000000394926889471</v>
+        <v>0.0000000104018836661</v>
       </c>
       <c r="L44" t="n">
-        <v>-1.20790999639</v>
+        <v>0.993763953092</v>
       </c>
       <c r="M44" t="n">
-        <v>0.227081884051644</v>
+        <v>0.320337799204316</v>
       </c>
       <c r="N44" t="n">
-        <v>0.486604037253523</v>
+        <v>0.667370415008992</v>
       </c>
     </row>
     <row r="45">
       <c r="A45" t="s">
-        <v>40</v>
+        <v>41</v>
       </c>
       <c r="B45" t="s">
-        <v>38</v>
+        <v>39</v>
       </c>
       <c r="C45" t="s">
         <v>35</v>
       </c>
       <c r="D45" t="n">
-        <v>0.0226034903615</v>
+        <v>0.0446037423259</v>
       </c>
       <c r="E45" t="n">
-        <v>0.00827550344364</v>
+        <v>0.049968372702</v>
       </c>
       <c r="F45" t="n">
-        <v>0.00857786411406</v>
+        <v>0.0202816420602</v>
       </c>
       <c r="G45" t="n">
-        <v>0.366116175479</v>
+        <v>1.12027310034</v>
       </c>
       <c r="H45" t="n">
-        <v>0.379492900294</v>
+        <v>0.454707183804</v>
       </c>
       <c r="I45" t="n">
-        <v>0.0869454278414295</v>
+        <v>0.792119617065983</v>
       </c>
       <c r="J45" t="n">
-        <v>-0.00000000177948855299</v>
+        <v>0.00000000263493921665</v>
       </c>
       <c r="K45" t="n">
-        <v>0.00000000106505790778</v>
+        <v>0.0000000051125010942</v>
       </c>
       <c r="L45" t="n">
-        <v>-1.67079042368</v>
+        <v>0.515391423512</v>
       </c>
       <c r="M45" t="n">
-        <v>0.0947630807229082</v>
+        <v>0.606279524425427</v>
       </c>
       <c r="N45" t="n">
-        <v>0.23690770180727</v>
+        <v>0.851724496542815</v>
       </c>
     </row>
     <row r="46">
       <c r="A46" t="s">
-        <v>40</v>
+        <v>41</v>
       </c>
       <c r="B46" t="s">
-        <v>38</v>
+        <v>39</v>
       </c>
       <c r="C46" t="s">
         <v>36</v>
       </c>
       <c r="D46" t="n">
+        <v>0.0376213753064</v>
+      </c>
+      <c r="E46" t="n">
+        <v>0.0848590507797</v>
+      </c>
+      <c r="F46" t="n">
+        <v>0.0305380845627</v>
+      </c>
+      <c r="G46" t="n">
+        <v>2.25560735323</v>
+      </c>
+      <c r="H46" t="n">
+        <v>0.811721642658</v>
+      </c>
+      <c r="I46" t="n">
+        <v>0.11360959248224</v>
+      </c>
+      <c r="J46" t="n">
+        <v>0.0000000189041996177</v>
+      </c>
+      <c r="K46" t="n">
+        <v>0.000000010731153725</v>
+      </c>
+      <c r="L46" t="n">
+        <v>1.76161856425</v>
+      </c>
+      <c r="M46" t="n">
+        <v>0.0781337652318049</v>
+      </c>
+      <c r="N46" t="n">
+        <v>0.218616775048539</v>
+      </c>
+    </row>
+    <row r="47">
+      <c r="A47" t="s">
+        <v>41</v>
+      </c>
+      <c r="B47" t="s">
+        <v>40</v>
+      </c>
+      <c r="C47" t="s">
+        <v>32</v>
+      </c>
+      <c r="D47" t="n">
+        <v>0.0415503092603</v>
+      </c>
+      <c r="E47" t="n">
+        <v>0.00749399654784</v>
+      </c>
+      <c r="F47" t="n">
+        <v>0.0202582461348</v>
+      </c>
+      <c r="G47" t="n">
+        <v>0.180359585313</v>
+      </c>
+      <c r="H47" t="n">
+        <v>0.487559454922</v>
+      </c>
+      <c r="I47" t="n">
+        <v>0.0874995154297556</v>
+      </c>
+      <c r="J47" t="n">
+        <v>-0.00000000374797725144</v>
+      </c>
+      <c r="K47" t="n">
+        <v>0.00000000558060062962</v>
+      </c>
+      <c r="L47" t="n">
+        <v>-0.671608219293</v>
+      </c>
+      <c r="M47" t="n">
+        <v>0.501833144332082</v>
+      </c>
+      <c r="N47" t="n">
+        <v>0.851724496542815</v>
+      </c>
+    </row>
+    <row r="48">
+      <c r="A48" t="s">
+        <v>41</v>
+      </c>
+      <c r="B48" t="s">
+        <v>40</v>
+      </c>
+      <c r="C48" t="s">
+        <v>33</v>
+      </c>
+      <c r="D48" t="n">
+        <v>0.0396572210203</v>
+      </c>
+      <c r="E48" t="n">
+        <v>0.049456324856</v>
+      </c>
+      <c r="F48" t="n">
+        <v>0.0363440358583</v>
+      </c>
+      <c r="G48" t="n">
+        <v>1.2470950708</v>
+      </c>
+      <c r="H48" t="n">
+        <v>0.916454429313</v>
+      </c>
+      <c r="I48" t="n">
+        <v>0.786279263480357</v>
+      </c>
+      <c r="J48" t="n">
+        <v>0.000000000299898416021</v>
+      </c>
+      <c r="K48" t="n">
+        <v>0.00000000994264571956</v>
+      </c>
+      <c r="L48" t="n">
+        <v>0.0301628383912</v>
+      </c>
+      <c r="M48" t="n">
+        <v>0.97593718570497</v>
+      </c>
+      <c r="N48" t="n">
+        <v>0.97593718570497</v>
+      </c>
+    </row>
+    <row r="49">
+      <c r="A49" t="s">
+        <v>41</v>
+      </c>
+      <c r="B49" t="s">
+        <v>40</v>
+      </c>
+      <c r="C49" t="s">
+        <v>34</v>
+      </c>
+      <c r="D49" t="n">
+        <v>0.055623243735</v>
+      </c>
+      <c r="E49" t="n">
+        <v>0.0895363072706</v>
+      </c>
+      <c r="F49" t="n">
+        <v>0.046941047451</v>
+      </c>
+      <c r="G49" t="n">
+        <v>1.60969230233</v>
+      </c>
+      <c r="H49" t="n">
+        <v>0.843910644166</v>
+      </c>
+      <c r="I49" t="n">
+        <v>0.458359672955946</v>
+      </c>
+      <c r="J49" t="n">
+        <v>0.0000000064996001484</v>
+      </c>
+      <c r="K49" t="n">
+        <v>0.00000000922254415378</v>
+      </c>
+      <c r="L49" t="n">
+        <v>0.704751318077</v>
+      </c>
+      <c r="M49" t="n">
+        <v>0.480965008998074</v>
+      </c>
+      <c r="N49" t="n">
+        <v>0.851724496542815</v>
+      </c>
+    </row>
+    <row r="50">
+      <c r="A50" t="s">
+        <v>41</v>
+      </c>
+      <c r="B50" t="s">
+        <v>40</v>
+      </c>
+      <c r="C50" t="s">
+        <v>35</v>
+      </c>
+      <c r="D50" t="n">
+        <v>0.0555658723413</v>
+      </c>
+      <c r="E50" t="n">
+        <v>0.0573961239559</v>
+      </c>
+      <c r="F50" t="n">
+        <v>0.0225672722456</v>
+      </c>
+      <c r="G50" t="n">
+        <v>1.03293841233</v>
+      </c>
+      <c r="H50" t="n">
+        <v>0.406135480192</v>
+      </c>
+      <c r="I50" t="n">
+        <v>0.935590694422955</v>
+      </c>
+      <c r="J50" t="n">
+        <v>0.00000000164572802611</v>
+      </c>
+      <c r="K50" t="n">
+        <v>0.00000000463591137525</v>
+      </c>
+      <c r="L50" t="n">
+        <v>0.354995575389</v>
+      </c>
+      <c r="M50" t="n">
+        <v>0.722592905972985</v>
+      </c>
+      <c r="N50" t="n">
+        <v>0.851724496542815</v>
+      </c>
+    </row>
+    <row r="51">
+      <c r="A51" t="s">
+        <v>41</v>
+      </c>
+      <c r="B51" t="s">
+        <v>40</v>
+      </c>
+      <c r="C51" t="s">
+        <v>36</v>
+      </c>
+      <c r="D51" t="n">
+        <v>0.0472146439979</v>
+      </c>
+      <c r="E51" t="n">
+        <v>0.106843377956</v>
+      </c>
+      <c r="F51" t="n">
+        <v>0.0346486638197</v>
+      </c>
+      <c r="G51" t="n">
+        <v>2.26292880575</v>
+      </c>
+      <c r="H51" t="n">
+        <v>0.73385417925</v>
+      </c>
+      <c r="I51" t="n">
+        <v>0.0752271671688956</v>
+      </c>
+      <c r="J51" t="n">
+        <v>0.0000000188319799384</v>
+      </c>
+      <c r="K51" t="n">
+        <v>0.00000000977542608526</v>
+      </c>
+      <c r="L51" t="n">
+        <v>1.92646128917</v>
+      </c>
+      <c r="M51" t="n">
+        <v>0.0540468009702292</v>
+      </c>
+      <c r="N51" t="n">
+        <v>0.215373239616491</v>
+      </c>
+    </row>
+    <row r="52">
+      <c r="A52" t="s">
+        <v>42</v>
+      </c>
+      <c r="B52" t="s">
+        <v>31</v>
+      </c>
+      <c r="C52" t="s">
+        <v>32</v>
+      </c>
+      <c r="D52" t="n">
+        <v>0.00799609606119</v>
+      </c>
+      <c r="E52" t="n">
+        <v>0.00222932693111</v>
+      </c>
+      <c r="F52" t="n">
+        <v>0.00339332996283</v>
+      </c>
+      <c r="G52" t="n">
+        <v>0.278801919593</v>
+      </c>
+      <c r="H52" t="n">
+        <v>0.424373336296</v>
+      </c>
+      <c r="I52" t="n">
+        <v>0.105506003223572</v>
+      </c>
+      <c r="J52" t="n">
+        <v>-0.000000000353836915763</v>
+      </c>
+      <c r="K52" t="n">
+        <v>0.00000000122853145732</v>
+      </c>
+      <c r="L52" t="n">
+        <v>-0.28801616243</v>
+      </c>
+      <c r="M52" t="n">
+        <v>0.773334366817085</v>
+      </c>
+      <c r="N52" t="n">
+        <v>0.955462226939499</v>
+      </c>
+    </row>
+    <row r="53">
+      <c r="A53" t="s">
+        <v>42</v>
+      </c>
+      <c r="B53" t="s">
+        <v>31</v>
+      </c>
+      <c r="C53" t="s">
+        <v>33</v>
+      </c>
+      <c r="D53" t="n">
+        <v>0.00866542898789</v>
+      </c>
+      <c r="E53" t="n">
+        <v>0.00463747352943</v>
+      </c>
+      <c r="F53" t="n">
+        <v>0.00981363042167</v>
+      </c>
+      <c r="G53" t="n">
+        <v>0.535169526623</v>
+      </c>
+      <c r="H53" t="n">
+        <v>1.13250370355</v>
+      </c>
+      <c r="I53" t="n">
+        <v>0.681186295423847</v>
+      </c>
+      <c r="J53" t="n">
+        <v>-0.00000000195003974656</v>
+      </c>
+      <c r="K53" t="n">
+        <v>0.00000000325972714089</v>
+      </c>
+      <c r="L53" t="n">
+        <v>-0.598221772031</v>
+      </c>
+      <c r="M53" t="n">
+        <v>0.54969196593028</v>
+      </c>
+      <c r="N53" t="n">
+        <v>0.763461063792055</v>
+      </c>
+    </row>
+    <row r="54">
+      <c r="A54" t="s">
+        <v>42</v>
+      </c>
+      <c r="B54" t="s">
+        <v>31</v>
+      </c>
+      <c r="C54" t="s">
+        <v>34</v>
+      </c>
+      <c r="D54" t="n">
+        <v>0.0113685945971</v>
+      </c>
+      <c r="E54" t="n">
+        <v>-0.0115931743094</v>
+      </c>
+      <c r="F54" t="n">
+        <v>0.0259534122571</v>
+      </c>
+      <c r="G54" t="n">
+        <v>-1.01975439535</v>
+      </c>
+      <c r="H54" t="n">
+        <v>2.28290419149</v>
+      </c>
+      <c r="I54" t="n">
+        <v>0.364636694422173</v>
+      </c>
+      <c r="J54" t="n">
+        <v>-0.00000000615026895169</v>
+      </c>
+      <c r="K54" t="n">
+        <v>0.00000000637836721396</v>
+      </c>
+      <c r="L54" t="n">
+        <v>-0.964238769168</v>
+      </c>
+      <c r="M54" t="n">
+        <v>0.334926231354079</v>
+      </c>
+      <c r="N54" t="n">
+        <v>0.558210385590131</v>
+      </c>
+    </row>
+    <row r="55">
+      <c r="A55" t="s">
+        <v>42</v>
+      </c>
+      <c r="B55" t="s">
+        <v>31</v>
+      </c>
+      <c r="C55" t="s">
+        <v>35</v>
+      </c>
+      <c r="D55" t="n">
+        <v>0.0111318956599</v>
+      </c>
+      <c r="E55" t="n">
+        <v>-0.000468572351367</v>
+      </c>
+      <c r="F55" t="n">
+        <v>0.0053618130074</v>
+      </c>
+      <c r="G55" t="n">
+        <v>-0.0420927724875</v>
+      </c>
+      <c r="H55" t="n">
+        <v>0.48166216889</v>
+      </c>
+      <c r="I55" t="n">
+        <v>0.025650039091221</v>
+      </c>
+      <c r="J55" t="n">
+        <v>-0.00000000297599351093</v>
+      </c>
+      <c r="K55" t="n">
+        <v>0.00000000134313478436</v>
+      </c>
+      <c r="L55" t="n">
+        <v>-2.21570727344</v>
+      </c>
+      <c r="M55" t="n">
+        <v>0.0267115564499915</v>
+      </c>
+      <c r="N55" t="n">
+        <v>0.111298151874965</v>
+      </c>
+    </row>
+    <row r="56">
+      <c r="A56" t="s">
+        <v>42</v>
+      </c>
+      <c r="B56" t="s">
+        <v>31</v>
+      </c>
+      <c r="C56" t="s">
+        <v>36</v>
+      </c>
+      <c r="D56" t="n">
+        <v>0.0091354718101</v>
+      </c>
+      <c r="E56" t="n">
+        <v>-0.0228530866343</v>
+      </c>
+      <c r="F56" t="n">
+        <v>0.0119125282179</v>
+      </c>
+      <c r="G56" t="n">
+        <v>-2.50157705145</v>
+      </c>
+      <c r="H56" t="n">
+        <v>1.30398609568</v>
+      </c>
+      <c r="I56" t="n">
+        <v>0.00273008378634463</v>
+      </c>
+      <c r="J56" t="n">
+        <v>-0.0000000111968500215</v>
+      </c>
+      <c r="K56" t="n">
+        <v>0.00000000350202355095</v>
+      </c>
+      <c r="L56" t="n">
+        <v>-3.19725149149</v>
+      </c>
+      <c r="M56" t="n">
+        <v>0.00138743903434683</v>
+      </c>
+      <c r="N56" t="n">
+        <v>0.0346859758586708</v>
+      </c>
+    </row>
+    <row r="57">
+      <c r="A57" t="s">
+        <v>42</v>
+      </c>
+      <c r="B57" t="s">
+        <v>37</v>
+      </c>
+      <c r="C57" t="s">
+        <v>32</v>
+      </c>
+      <c r="D57" t="n">
+        <v>0.0158392017391</v>
+      </c>
+      <c r="E57" t="n">
+        <v>0.00910884541401</v>
+      </c>
+      <c r="F57" t="n">
+        <v>0.00590761807635</v>
+      </c>
+      <c r="G57" t="n">
+        <v>0.57508235352</v>
+      </c>
+      <c r="H57" t="n">
+        <v>0.372974482783</v>
+      </c>
+      <c r="I57" t="n">
+        <v>0.265817083546758</v>
+      </c>
+      <c r="J57" t="n">
+        <v>0.00000000021986460267</v>
+      </c>
+      <c r="K57" t="n">
+        <v>0.00000000112813483351</v>
+      </c>
+      <c r="L57" t="n">
+        <v>0.194892131809</v>
+      </c>
+      <c r="M57" t="n">
+        <v>0.84547739399404</v>
+      </c>
+      <c r="N57" t="n">
+        <v>0.955462226939499</v>
+      </c>
+    </row>
+    <row r="58">
+      <c r="A58" t="s">
+        <v>42</v>
+      </c>
+      <c r="B58" t="s">
+        <v>37</v>
+      </c>
+      <c r="C58" t="s">
+        <v>33</v>
+      </c>
+      <c r="D58" t="n">
+        <v>0.0170143087946</v>
+      </c>
+      <c r="E58" t="n">
+        <v>0.0189647884069</v>
+      </c>
+      <c r="F58" t="n">
+        <v>0.0150771954148</v>
+      </c>
+      <c r="G58" t="n">
+        <v>1.11463760508</v>
+      </c>
+      <c r="H58" t="n">
+        <v>0.886147982667</v>
+      </c>
+      <c r="I58" t="n">
+        <v>0.896507651971053</v>
+      </c>
+      <c r="J58" t="n">
+        <v>-0.000000000219238920646</v>
+      </c>
+      <c r="K58" t="n">
+        <v>0.00000000255838368877</v>
+      </c>
+      <c r="L58" t="n">
+        <v>-0.0856943083277</v>
+      </c>
+      <c r="M58" t="n">
+        <v>0.931709426782296</v>
+      </c>
+      <c r="N58" t="n">
+        <v>0.955462226939499</v>
+      </c>
+    </row>
+    <row r="59">
+      <c r="A59" t="s">
+        <v>42</v>
+      </c>
+      <c r="B59" t="s">
+        <v>37</v>
+      </c>
+      <c r="C59" t="s">
+        <v>34</v>
+      </c>
+      <c r="D59" t="n">
+        <v>0.0224921026264</v>
+      </c>
+      <c r="E59" t="n">
+        <v>-0.0116710750391</v>
+      </c>
+      <c r="F59" t="n">
+        <v>0.031391513915</v>
+      </c>
+      <c r="G59" t="n">
+        <v>-0.518896575965</v>
+      </c>
+      <c r="H59" t="n">
+        <v>1.39566826795</v>
+      </c>
+      <c r="I59" t="n">
+        <v>0.265776393859218</v>
+      </c>
+      <c r="J59" t="n">
+        <v>-0.00000000477036137637</v>
+      </c>
+      <c r="K59" t="n">
+        <v>0.00000000394926889471</v>
+      </c>
+      <c r="L59" t="n">
+        <v>-1.20790999639</v>
+      </c>
+      <c r="M59" t="n">
+        <v>0.227081884051644</v>
+      </c>
+      <c r="N59" t="n">
+        <v>0.426106059527445</v>
+      </c>
+    </row>
+    <row r="60">
+      <c r="A60" t="s">
+        <v>42</v>
+      </c>
+      <c r="B60" t="s">
+        <v>37</v>
+      </c>
+      <c r="C60" t="s">
+        <v>35</v>
+      </c>
+      <c r="D60" t="n">
+        <v>0.0226034903615</v>
+      </c>
+      <c r="E60" t="n">
+        <v>0.00827550344364</v>
+      </c>
+      <c r="F60" t="n">
+        <v>0.00857786411406</v>
+      </c>
+      <c r="G60" t="n">
+        <v>0.366116175479</v>
+      </c>
+      <c r="H60" t="n">
+        <v>0.379492900294</v>
+      </c>
+      <c r="I60" t="n">
+        <v>0.0869454278414295</v>
+      </c>
+      <c r="J60" t="n">
+        <v>-0.00000000177948855299</v>
+      </c>
+      <c r="K60" t="n">
+        <v>0.00000000106505790778</v>
+      </c>
+      <c r="L60" t="n">
+        <v>-1.67079042368</v>
+      </c>
+      <c r="M60" t="n">
+        <v>0.0947630807229082</v>
+      </c>
+      <c r="N60" t="n">
+        <v>0.263230779785856</v>
+      </c>
+    </row>
+    <row r="61">
+      <c r="A61" t="s">
+        <v>42</v>
+      </c>
+      <c r="B61" t="s">
+        <v>37</v>
+      </c>
+      <c r="C61" t="s">
+        <v>36</v>
+      </c>
+      <c r="D61" t="n">
         <v>0.0185626654146</v>
       </c>
-      <c r="E46" t="n">
+      <c r="E61" t="n">
         <v>-0.0229370693941</v>
       </c>
-      <c r="F46" t="n">
+      <c r="F61" t="n">
         <v>0.0173606003799</v>
       </c>
-      <c r="G46" t="n">
+      <c r="G61" t="n">
         <v>-1.23565602686</v>
       </c>
-      <c r="H46" t="n">
+      <c r="H61" t="n">
         <v>0.935242864761</v>
       </c>
-      <c r="I46" t="n">
+      <c r="I61" t="n">
         <v>0.0131479470546408</v>
       </c>
-      <c r="J46" t="n">
+      <c r="J61" t="n">
         <v>-0.00000000778012845204</v>
       </c>
-      <c r="K46" t="n">
+      <c r="K61" t="n">
         <v>0.00000000286149470728</v>
       </c>
-      <c r="L46" t="n">
+      <c r="L61" t="n">
         <v>-2.71890366676</v>
       </c>
-      <c r="M46" t="n">
+      <c r="M61" t="n">
         <v>0.00654986807929461</v>
       </c>
-      <c r="N46" t="n">
-        <v>0.0441569204065925</v>
+      <c r="N61" t="n">
+        <v>0.0425920883887166</v>
+      </c>
+    </row>
+    <row r="62">
+      <c r="A62" t="s">
+        <v>42</v>
+      </c>
+      <c r="B62" t="s">
+        <v>38</v>
+      </c>
+      <c r="C62" t="s">
+        <v>32</v>
+      </c>
+      <c r="D62" t="n">
+        <v>0.0245074825214</v>
+      </c>
+      <c r="E62" t="n">
+        <v>0.013851519739</v>
+      </c>
+      <c r="F62" t="n">
+        <v>0.00736106637038</v>
+      </c>
+      <c r="G62" t="n">
+        <v>0.565195536788</v>
+      </c>
+      <c r="H62" t="n">
+        <v>0.300359955942</v>
+      </c>
+      <c r="I62" t="n">
+        <v>0.158186717469599</v>
+      </c>
+      <c r="J62" t="n">
+        <v>-0.0000000000729358635913</v>
+      </c>
+      <c r="K62" t="n">
+        <v>0.000000000895913525701</v>
+      </c>
+      <c r="L62" t="n">
+        <v>-0.0814094904241</v>
+      </c>
+      <c r="M62" t="n">
+        <v>0.93511630189756</v>
+      </c>
+      <c r="N62" t="n">
+        <v>0.955462226939499</v>
+      </c>
+    </row>
+    <row r="63">
+      <c r="A63" t="s">
+        <v>42</v>
+      </c>
+      <c r="B63" t="s">
+        <v>38</v>
+      </c>
+      <c r="C63" t="s">
+        <v>33</v>
+      </c>
+      <c r="D63" t="n">
+        <v>0.0249590725562</v>
+      </c>
+      <c r="E63" t="n">
+        <v>0.0279855164347</v>
+      </c>
+      <c r="F63" t="n">
+        <v>0.0186859520863</v>
+      </c>
+      <c r="G63" t="n">
+        <v>1.1212562635</v>
+      </c>
+      <c r="H63" t="n">
+        <v>0.748663719142</v>
+      </c>
+      <c r="I63" t="n">
+        <v>0.870730857203132</v>
+      </c>
+      <c r="J63" t="n">
+        <v>-0.000000000121472905231</v>
+      </c>
+      <c r="K63" t="n">
+        <v>0.00000000217503004965</v>
+      </c>
+      <c r="L63" t="n">
+        <v>-0.0558488399965</v>
+      </c>
+      <c r="M63" t="n">
+        <v>0.955462226939499</v>
+      </c>
+      <c r="N63" t="n">
+        <v>0.955462226939499</v>
+      </c>
+    </row>
+    <row r="64">
+      <c r="A64" t="s">
+        <v>42</v>
+      </c>
+      <c r="B64" t="s">
+        <v>38</v>
+      </c>
+      <c r="C64" t="s">
+        <v>34</v>
+      </c>
+      <c r="D64" t="n">
+        <v>0.0335382767009</v>
+      </c>
+      <c r="E64" t="n">
+        <v>-0.0151665337067</v>
+      </c>
+      <c r="F64" t="n">
+        <v>0.0345307407664</v>
+      </c>
+      <c r="G64" t="n">
+        <v>-0.452215653236</v>
+      </c>
+      <c r="H64" t="n">
+        <v>1.02959198156</v>
+      </c>
+      <c r="I64" t="n">
+        <v>0.147279776754031</v>
+      </c>
+      <c r="J64" t="n">
+        <v>-0.00000000463641054663</v>
+      </c>
+      <c r="K64" t="n">
+        <v>0.00000000293407462899</v>
+      </c>
+      <c r="L64" t="n">
+        <v>-1.58019516642</v>
+      </c>
+      <c r="M64" t="n">
+        <v>0.114062178382343</v>
+      </c>
+      <c r="N64" t="n">
+        <v>0.285155445955859</v>
+      </c>
+    </row>
+    <row r="65">
+      <c r="A65" t="s">
+        <v>42</v>
+      </c>
+      <c r="B65" t="s">
+        <v>38</v>
+      </c>
+      <c r="C65" t="s">
+        <v>35</v>
+      </c>
+      <c r="D65" t="n">
+        <v>0.0336612393664</v>
+      </c>
+      <c r="E65" t="n">
+        <v>0.0187195200662</v>
+      </c>
+      <c r="F65" t="n">
+        <v>0.0113830171227</v>
+      </c>
+      <c r="G65" t="n">
+        <v>0.556114998097</v>
+      </c>
+      <c r="H65" t="n">
+        <v>0.33816393386</v>
+      </c>
+      <c r="I65" t="n">
+        <v>0.177724335989853</v>
+      </c>
+      <c r="J65" t="n">
+        <v>-0.00000000110226827198</v>
+      </c>
+      <c r="K65" t="n">
+        <v>0.000000000935358558229</v>
+      </c>
+      <c r="L65" t="n">
+        <v>-1.17844463204</v>
+      </c>
+      <c r="M65" t="n">
+        <v>0.238619393335369</v>
+      </c>
+      <c r="N65" t="n">
+        <v>0.426106059527445</v>
+      </c>
+    </row>
+    <row r="66">
+      <c r="A66" t="s">
+        <v>42</v>
+      </c>
+      <c r="B66" t="s">
+        <v>38</v>
+      </c>
+      <c r="C66" t="s">
+        <v>36</v>
+      </c>
+      <c r="D66" t="n">
+        <v>0.0279980788971</v>
+      </c>
+      <c r="E66" t="n">
+        <v>-0.0225722554113</v>
+      </c>
+      <c r="F66" t="n">
+        <v>0.020828780134</v>
+      </c>
+      <c r="G66" t="n">
+        <v>-0.806207293519</v>
+      </c>
+      <c r="H66" t="n">
+        <v>0.743936046848</v>
+      </c>
+      <c r="I66" t="n">
+        <v>0.0156568487251507</v>
+      </c>
+      <c r="J66" t="n">
+        <v>-0.00000000677239099422</v>
+      </c>
+      <c r="K66" t="n">
+        <v>0.00000000243278175328</v>
+      </c>
+      <c r="L66" t="n">
+        <v>-2.7838054051</v>
+      </c>
+      <c r="M66" t="n">
+        <v>0.00537252563989595</v>
+      </c>
+      <c r="N66" t="n">
+        <v>0.0425920883887166</v>
+      </c>
+    </row>
+    <row r="67">
+      <c r="A67" t="s">
+        <v>42</v>
+      </c>
+      <c r="B67" t="s">
+        <v>39</v>
+      </c>
+      <c r="C67" t="s">
+        <v>32</v>
+      </c>
+      <c r="D67" t="n">
+        <v>0.0330351866139</v>
+      </c>
+      <c r="E67" t="n">
+        <v>0.0144781487036</v>
+      </c>
+      <c r="F67" t="n">
+        <v>0.00842263717171</v>
+      </c>
+      <c r="G67" t="n">
+        <v>0.438264474568</v>
+      </c>
+      <c r="H67" t="n">
+        <v>0.254959575987</v>
+      </c>
+      <c r="I67" t="n">
+        <v>0.034949566146374</v>
+      </c>
+      <c r="J67" t="n">
+        <v>-0.000000000564758510586</v>
+      </c>
+      <c r="K67" t="n">
+        <v>0.000000000781343283914</v>
+      </c>
+      <c r="L67" t="n">
+        <v>-0.722804588217</v>
+      </c>
+      <c r="M67" t="n">
+        <v>0.469799948069094</v>
+      </c>
+      <c r="N67" t="n">
+        <v>0.690882276572198</v>
+      </c>
+    </row>
+    <row r="68">
+      <c r="A68" t="s">
+        <v>42</v>
+      </c>
+      <c r="B68" t="s">
+        <v>39</v>
+      </c>
+      <c r="C68" t="s">
+        <v>33</v>
+      </c>
+      <c r="D68" t="n">
+        <v>0.0325320965269</v>
+      </c>
+      <c r="E68" t="n">
+        <v>0.0359301061501</v>
+      </c>
+      <c r="F68" t="n">
+        <v>0.021343379758</v>
+      </c>
+      <c r="G68" t="n">
+        <v>1.10445098798</v>
+      </c>
+      <c r="H68" t="n">
+        <v>0.656071450554</v>
+      </c>
+      <c r="I68" t="n">
+        <v>0.872928933426051</v>
+      </c>
+      <c r="J68" t="n">
+        <v>-0.000000000122248999193</v>
+      </c>
+      <c r="K68" t="n">
+        <v>0.00000000192262640085</v>
+      </c>
+      <c r="L68" t="n">
+        <v>-0.0635843755911</v>
+      </c>
+      <c r="M68" t="n">
+        <v>0.949301173036987</v>
+      </c>
+      <c r="N68" t="n">
+        <v>0.955462226939499</v>
+      </c>
+    </row>
+    <row r="69">
+      <c r="A69" t="s">
+        <v>42</v>
+      </c>
+      <c r="B69" t="s">
+        <v>39</v>
+      </c>
+      <c r="C69" t="s">
+        <v>34</v>
+      </c>
+      <c r="D69" t="n">
+        <v>0.0445886445908</v>
+      </c>
+      <c r="E69" t="n">
+        <v>-0.0190807342829</v>
+      </c>
+      <c r="F69" t="n">
+        <v>0.0377350541039</v>
+      </c>
+      <c r="G69" t="n">
+        <v>-0.427928107213</v>
+      </c>
+      <c r="H69" t="n">
+        <v>0.846292917183</v>
+      </c>
+      <c r="I69" t="n">
+        <v>0.0815612340358276</v>
+      </c>
+      <c r="J69" t="n">
+        <v>-0.00000000461457178441</v>
+      </c>
+      <c r="K69" t="n">
+        <v>0.00000000243813154906</v>
+      </c>
+      <c r="L69" t="n">
+        <v>-1.89266727064</v>
+      </c>
+      <c r="M69" t="n">
+        <v>0.0584021315543463</v>
+      </c>
+      <c r="N69" t="n">
+        <v>0.182506661107332</v>
+      </c>
+    </row>
+    <row r="70">
+      <c r="A70" t="s">
+        <v>42</v>
+      </c>
+      <c r="B70" t="s">
+        <v>39</v>
+      </c>
+      <c r="C70" t="s">
+        <v>35</v>
+      </c>
+      <c r="D70" t="n">
+        <v>0.0446037423259</v>
+      </c>
+      <c r="E70" t="n">
+        <v>0.0231253326404</v>
+      </c>
+      <c r="F70" t="n">
+        <v>0.0142099118881</v>
+      </c>
+      <c r="G70" t="n">
+        <v>0.518461712729</v>
+      </c>
+      <c r="H70" t="n">
+        <v>0.318581158152</v>
+      </c>
+      <c r="I70" t="n">
+        <v>0.114819721310444</v>
+      </c>
+      <c r="J70" t="n">
+        <v>-0.00000000123213629421</v>
+      </c>
+      <c r="K70" t="n">
+        <v>0.00000000085483157962</v>
+      </c>
+      <c r="L70" t="n">
+        <v>-1.44137900796</v>
+      </c>
+      <c r="M70" t="n">
+        <v>0.149477637472921</v>
+      </c>
+      <c r="N70" t="n">
+        <v>0.339721903347547</v>
+      </c>
+    </row>
+    <row r="71">
+      <c r="A71" t="s">
+        <v>42</v>
+      </c>
+      <c r="B71" t="s">
+        <v>39</v>
+      </c>
+      <c r="C71" t="s">
+        <v>36</v>
+      </c>
+      <c r="D71" t="n">
+        <v>0.0376213753064</v>
+      </c>
+      <c r="E71" t="n">
+        <v>-0.0181707702966</v>
+      </c>
+      <c r="F71" t="n">
+        <v>0.0240759371114</v>
+      </c>
+      <c r="G71" t="n">
+        <v>-0.482990591084</v>
+      </c>
+      <c r="H71" t="n">
+        <v>0.639953667706</v>
+      </c>
+      <c r="I71" t="n">
+        <v>0.0217362015609925</v>
+      </c>
+      <c r="J71" t="n">
+        <v>-0.00000000589010501849</v>
+      </c>
+      <c r="K71" t="n">
+        <v>0.00000000217687270316</v>
+      </c>
+      <c r="L71" t="n">
+        <v>-2.70576456305</v>
+      </c>
+      <c r="M71" t="n">
+        <v>0.00681473414219466</v>
+      </c>
+      <c r="N71" t="n">
+        <v>0.0425920883887166</v>
+      </c>
+    </row>
+    <row r="72">
+      <c r="A72" t="s">
+        <v>42</v>
+      </c>
+      <c r="B72" t="s">
+        <v>40</v>
+      </c>
+      <c r="C72" t="s">
+        <v>32</v>
+      </c>
+      <c r="D72" t="n">
+        <v>0.0415503092603</v>
+      </c>
+      <c r="E72" t="n">
+        <v>0.0184207219789</v>
+      </c>
+      <c r="F72" t="n">
+        <v>0.0104327122914</v>
+      </c>
+      <c r="G72" t="n">
+        <v>0.443335376</v>
+      </c>
+      <c r="H72" t="n">
+        <v>0.251086272932</v>
+      </c>
+      <c r="I72" t="n">
+        <v>0.0308419832660619</v>
+      </c>
+      <c r="J72" t="n">
+        <v>-0.000000000712503811255</v>
+      </c>
+      <c r="K72" t="n">
+        <v>0.000000000779192457209</v>
+      </c>
+      <c r="L72" t="n">
+        <v>-0.914413126902</v>
+      </c>
+      <c r="M72" t="n">
+        <v>0.360499806791728</v>
+      </c>
+      <c r="N72" t="n">
+        <v>0.563280948112075</v>
+      </c>
+    </row>
+    <row r="73">
+      <c r="A73" t="s">
+        <v>42</v>
+      </c>
+      <c r="B73" t="s">
+        <v>40</v>
+      </c>
+      <c r="C73" t="s">
+        <v>33</v>
+      </c>
+      <c r="D73" t="n">
+        <v>0.0396572210203</v>
+      </c>
+      <c r="E73" t="n">
+        <v>0.0430535635417</v>
+      </c>
+      <c r="F73" t="n">
+        <v>0.0241293424324</v>
+      </c>
+      <c r="G73" t="n">
+        <v>1.08564247403</v>
+      </c>
+      <c r="H73" t="n">
+        <v>0.608447637319</v>
+      </c>
+      <c r="I73" t="n">
+        <v>0.887418738114685</v>
+      </c>
+      <c r="J73" t="n">
+        <v>-0.000000000128468127844</v>
+      </c>
+      <c r="K73" t="n">
+        <v>0.00000000179183733796</v>
+      </c>
+      <c r="L73" t="n">
+        <v>-0.0716963114468</v>
+      </c>
+      <c r="M73" t="n">
+        <v>0.942843591649055</v>
+      </c>
+      <c r="N73" t="n">
+        <v>0.955462226939499</v>
+      </c>
+    </row>
+    <row r="74">
+      <c r="A74" t="s">
+        <v>42</v>
+      </c>
+      <c r="B74" t="s">
+        <v>40</v>
+      </c>
+      <c r="C74" t="s">
+        <v>34</v>
+      </c>
+      <c r="D74" t="n">
+        <v>0.055623243735</v>
+      </c>
+      <c r="E74" t="n">
+        <v>-0.0173039343952</v>
+      </c>
+      <c r="F74" t="n">
+        <v>0.0408024573047</v>
+      </c>
+      <c r="G74" t="n">
+        <v>-0.31109178885</v>
+      </c>
+      <c r="H74" t="n">
+        <v>0.733550482943</v>
+      </c>
+      <c r="I74" t="n">
+        <v>0.0666633175428206</v>
+      </c>
+      <c r="J74" t="n">
+        <v>-0.00000000431267545276</v>
+      </c>
+      <c r="K74" t="n">
+        <v>0.00000000215837202486</v>
+      </c>
+      <c r="L74" t="n">
+        <v>-1.99811496957</v>
+      </c>
+      <c r="M74" t="n">
+        <v>0.0457041971842485</v>
+      </c>
+      <c r="N74" t="n">
+        <v>0.16322927565803</v>
+      </c>
+    </row>
+    <row r="75">
+      <c r="A75" t="s">
+        <v>42</v>
+      </c>
+      <c r="B75" t="s">
+        <v>40</v>
+      </c>
+      <c r="C75" t="s">
+        <v>35</v>
+      </c>
+      <c r="D75" t="n">
+        <v>0.0555658723413</v>
+      </c>
+      <c r="E75" t="n">
+        <v>0.0318535451979</v>
+      </c>
+      <c r="F75" t="n">
+        <v>0.0174655201519</v>
+      </c>
+      <c r="G75" t="n">
+        <v>0.573257358442</v>
+      </c>
+      <c r="H75" t="n">
+        <v>0.314320992652</v>
+      </c>
+      <c r="I75" t="n">
+        <v>0.155294326870042</v>
+      </c>
+      <c r="J75" t="n">
+        <v>-0.00000000106255471002</v>
+      </c>
+      <c r="K75" t="n">
+        <v>0.000000000833741169373</v>
+      </c>
+      <c r="L75" t="n">
+        <v>-1.274441936</v>
+      </c>
+      <c r="M75" t="n">
+        <v>0.202506838187046</v>
+      </c>
+      <c r="N75" t="n">
+        <v>0.421889246223013</v>
+      </c>
+    </row>
+    <row r="76">
+      <c r="A76" t="s">
+        <v>42</v>
+      </c>
+      <c r="B76" t="s">
+        <v>40</v>
+      </c>
+      <c r="C76" t="s">
+        <v>36</v>
+      </c>
+      <c r="D76" t="n">
+        <v>0.0472146439979</v>
+      </c>
+      <c r="E76" t="n">
+        <v>-0.00609669369846</v>
+      </c>
+      <c r="F76" t="n">
+        <v>0.0261143488837</v>
+      </c>
+      <c r="G76" t="n">
+        <v>-0.129127177126</v>
+      </c>
+      <c r="H76" t="n">
+        <v>0.553098502338</v>
+      </c>
+      <c r="I76" t="n">
+        <v>0.0455315480201227</v>
+      </c>
+      <c r="J76" t="n">
+        <v>-0.00000000485945547692</v>
+      </c>
+      <c r="K76" t="n">
+        <v>0.00000000194441567112</v>
+      </c>
+      <c r="L76" t="n">
+        <v>-2.49918551321</v>
+      </c>
+      <c r="M76" t="n">
+        <v>0.0124479128767305</v>
+      </c>
+      <c r="N76" t="n">
+        <v>0.0622395643836524</v>
       </c>
     </row>
   </sheetData>

</xml_diff>